<commit_message>
TS 1.1 Jatai Ghanam files 25/07/2021
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Padam Input Templates/TS 4.7 Padam Input Template.xlsx
+++ b/TS Jatai Working/Padam Input Templates/TS 4.7 Padam Input Template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\texts\TS Jatai Working\Raja Files\Padam Inputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\texts\TS Jatai Working\Padam Input Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{165FA615-F2AC-4CBD-A4A7-DF09E45B825B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7614CE16-BECD-4659-A8EC-E535E09AE54D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4731,10 +4731,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W2010"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A242" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2000" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="H1" sqref="H1"/>
-      <selection pane="bottomLeft" activeCell="V243" sqref="V243"/>
+      <selection pane="bottomLeft" activeCell="H243" sqref="H243"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
TS 1.1 Jatai files edited and new created 26/07/2021
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Padam Input Templates/TS 4.7 Padam Input Template.xlsx
+++ b/TS Jatai Working/Padam Input Templates/TS 4.7 Padam Input Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\texts\TS Jatai Working\Padam Input Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7614CE16-BECD-4659-A8EC-E535E09AE54D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E15AD72-AAA8-4FDF-A305-B642BC1E363F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4731,10 +4731,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W2010"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2000" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A1448" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="H1" sqref="H1"/>
-      <selection pane="bottomLeft" activeCell="H243" sqref="H243"/>
+      <selection pane="bottomLeft" activeCell="I1446" sqref="I1446"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
TS 1.6 Jatai Ghanam Tamil 28/03/2022
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Padam Input Templates/TS 4.7 Padam Input Template.xlsx
+++ b/TS Jatai Working/Padam Input Templates/TS 4.7 Padam Input Template.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Documents\GitHub\texts\TS Jatai Working\Padam Input Templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\texts\TS Jatai Working\Padam Input Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{271DD81E-F4F2-4E18-A0D3-297DD2010387}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TS 4.7" sheetId="1" r:id="rId1"/>
@@ -17,10 +18,18 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'TS 4.7'!$S$2001:$S$2001</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -4055,7 +4064,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -4727,13 +4736,13 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W2010"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="N1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A1547" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="H1" sqref="H1"/>
-      <selection pane="bottomLeft" activeCell="S1558" sqref="S1558"/>
+      <selection pane="bottomLeft" activeCell="V1" sqref="V1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -75937,11 +75946,11 @@
       <c r="C2010" s="49"/>
     </row>
   </sheetData>
-  <autoFilter ref="S2001"/>
+  <autoFilter ref="S2001" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <hyperlinks>
-    <hyperlink ref="N1223" r:id="rId1" display="a@Bi"/>
-    <hyperlink ref="N1233" r:id="rId2" display="a@Bi"/>
-    <hyperlink ref="N1242" r:id="rId3" display="a@Bi"/>
+    <hyperlink ref="N1223" r:id="rId1" display="a@Bi" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="N1233" r:id="rId2" display="a@Bi" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="N1242" r:id="rId3" display="a@Bi" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId4"/>

</xml_diff>

<commit_message>
nmv 28 02 2023
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Padam Input Templates/TS 4.7 Padam Input Template.xlsx
+++ b/TS Jatai Working/Padam Input Templates/TS 4.7 Padam Input Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ALL IMP DATA\GitHub\texts\TS Jatai Working\Padam Input Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E469D548-B3D9-4026-97FF-4DE55DB7236E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AB43EF1-5534-416A-8A97-7FE2D913886C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4257,7 +4257,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -4426,35 +4426,22 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4735,12 +4722,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W2010"/>
+  <dimension ref="A1:AA2010"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="I1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A438" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A1994" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="H1" sqref="H1"/>
-      <selection pane="bottomLeft" activeCell="N455" sqref="N455:V455"/>
+      <selection pane="bottomLeft" activeCell="N2012" sqref="N2012"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -20625,7 +20612,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="449" spans="5:22" s="6" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="449" spans="5:27" s="6" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I449" s="52" t="s">
         <v>695</v>
       </c>
@@ -20658,7 +20645,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="450" spans="5:22" s="6" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="450" spans="5:27" s="6" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I450" s="52" t="s">
         <v>695</v>
       </c>
@@ -20691,7 +20678,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="451" spans="5:22" s="6" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="451" spans="5:27" s="6" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I451" s="52" t="s">
         <v>695</v>
       </c>
@@ -20724,7 +20711,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="452" spans="5:22" s="6" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="452" spans="5:27" s="6" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I452" s="52" t="s">
         <v>695</v>
       </c>
@@ -20757,7 +20744,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="453" spans="5:22" s="6" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="453" spans="5:27" s="6" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I453" s="52" t="s">
         <v>695</v>
       </c>
@@ -20790,7 +20777,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="454" spans="5:22" s="6" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="454" spans="5:27" s="6" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I454" s="52" t="s">
         <v>695</v>
       </c>
@@ -20823,7 +20810,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="455" spans="5:22" s="6" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="455" spans="5:27" s="6" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I455" s="52" t="s">
         <v>695</v>
       </c>
@@ -20842,23 +20829,28 @@
         <f t="shared" si="51"/>
         <v>114</v>
       </c>
-      <c r="N455" s="69" t="s">
+      <c r="N455" s="63" t="s">
         <v>1159</v>
       </c>
-      <c r="O455" s="70"/>
-      <c r="P455" s="70" t="s">
+      <c r="O455" s="64"/>
+      <c r="P455" s="64" t="s">
         <v>18</v>
       </c>
-      <c r="Q455" s="71"/>
-      <c r="R455" s="71"/>
-      <c r="S455" s="71"/>
-      <c r="T455" s="71"/>
-      <c r="U455" s="71"/>
-      <c r="V455" s="72" t="s">
+      <c r="Q455" s="65"/>
+      <c r="R455" s="65"/>
+      <c r="S455" s="65"/>
+      <c r="T455" s="65"/>
+      <c r="U455" s="65"/>
+      <c r="V455" s="66" t="s">
         <v>1247</v>
       </c>
-    </row>
-    <row r="456" spans="5:22" s="6" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="W455" s="67"/>
+      <c r="X455" s="67"/>
+      <c r="Y455" s="67"/>
+      <c r="Z455" s="67"/>
+      <c r="AA455" s="67"/>
+    </row>
+    <row r="456" spans="5:27" s="6" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I456" s="52" t="s">
         <v>696</v>
       </c>
@@ -20889,7 +20881,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="457" spans="5:22" s="6" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="457" spans="5:27" s="6" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I457" s="52" t="s">
         <v>696</v>
       </c>
@@ -20922,7 +20914,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="458" spans="5:22" s="6" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="458" spans="5:27" s="6" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I458" s="52" t="s">
         <v>696</v>
       </c>
@@ -20955,7 +20947,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="459" spans="5:22" s="6" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="459" spans="5:27" s="6" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I459" s="52" t="s">
         <v>696</v>
       </c>
@@ -20988,7 +20980,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="460" spans="5:22" s="6" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="460" spans="5:27" s="6" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E460" s="14"/>
       <c r="I460" s="52" t="s">
         <v>696</v>
@@ -21022,7 +21014,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="461" spans="5:22" s="6" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="461" spans="5:27" s="6" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E461" s="14"/>
       <c r="I461" s="52" t="s">
         <v>696</v>
@@ -21056,7 +21048,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="462" spans="5:22" s="6" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="462" spans="5:27" s="6" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I462" s="52" t="s">
         <v>696</v>
       </c>
@@ -21089,7 +21081,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="463" spans="5:22" s="6" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="463" spans="5:27" s="6" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I463" s="52" t="s">
         <v>696</v>
       </c>
@@ -21122,7 +21114,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="464" spans="5:22" s="6" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="464" spans="5:27" s="6" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I464" s="52" t="s">
         <v>696</v>
       </c>
@@ -49663,7 +49655,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="1281" spans="1:23" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1281" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1281" s="44" t="s">
         <v>1150</v>
       </c>
@@ -49702,7 +49694,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="1282" spans="1:23" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1282" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1282" s="44" t="s">
         <v>1150</v>
       </c>
@@ -49743,7 +49735,7 @@
         <v>1268</v>
       </c>
     </row>
-    <row r="1283" spans="1:23" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1283" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1283" s="44" t="s">
         <v>1150</v>
       </c>
@@ -49782,7 +49774,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="1284" spans="1:23" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1284" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1284" s="44" t="s">
         <v>1150</v>
       </c>
@@ -49821,7 +49813,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="1285" spans="1:23" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1285" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1285" s="44" t="s">
         <v>1150</v>
       </c>
@@ -49862,7 +49854,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="1286" spans="1:23" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1286" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1286" s="44" t="s">
         <v>1150</v>
       </c>
@@ -49901,7 +49893,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="1287" spans="1:23" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1287" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1287" s="44" t="s">
         <v>1150</v>
       </c>
@@ -49940,7 +49932,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="1288" spans="1:23" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1288" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1288" s="44" t="s">
         <v>1150</v>
       </c>
@@ -49979,7 +49971,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="1289" spans="1:23" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1289" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1289" s="44" t="s">
         <v>1150</v>
       </c>
@@ -50022,7 +50014,7 @@
         <v>1269</v>
       </c>
     </row>
-    <row r="1290" spans="1:23" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1290" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1290" s="44" t="s">
         <v>1150</v>
       </c>
@@ -50063,7 +50055,7 @@
         <v>1001</v>
       </c>
     </row>
-    <row r="1291" spans="1:23" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1291" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1291" s="44" t="s">
         <v>1150</v>
       </c>
@@ -50102,7 +50094,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="1292" spans="1:23" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1292" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1292" s="44" t="s">
         <v>1150</v>
       </c>
@@ -50141,7 +50133,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="1293" spans="1:23" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1293" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1293" s="44" t="s">
         <v>1150</v>
       </c>
@@ -50180,7 +50172,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="1294" spans="1:23" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1294" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1294" s="44" t="s">
         <v>1150</v>
       </c>
@@ -50221,7 +50213,7 @@
         <v>1002</v>
       </c>
     </row>
-    <row r="1295" spans="1:23" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1295" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1295" s="44" t="s">
         <v>1150</v>
       </c>
@@ -50246,22 +50238,21 @@
         <f t="shared" si="82"/>
         <v>50</v>
       </c>
-      <c r="N1295" s="62" t="s">
+      <c r="N1295" s="21" t="s">
         <v>217</v>
       </c>
-      <c r="O1295" s="63"/>
-      <c r="P1295" s="64"/>
-      <c r="Q1295" s="65"/>
-      <c r="R1295" s="65"/>
-      <c r="S1295" s="65"/>
-      <c r="T1295" s="65"/>
-      <c r="U1295" s="65"/>
-      <c r="V1295" s="66" t="s">
-        <v>727</v>
-      </c>
-      <c r="W1295" s="67"/>
-    </row>
-    <row r="1296" spans="1:23" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O1295" s="23"/>
+      <c r="P1295" s="24"/>
+      <c r="Q1295" s="8"/>
+      <c r="R1295" s="8"/>
+      <c r="S1295" s="8"/>
+      <c r="T1295" s="8"/>
+      <c r="U1295" s="8"/>
+      <c r="V1295" s="5" t="s">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="1296" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1296" s="44" t="s">
         <v>1150</v>
       </c>
@@ -54788,7 +54779,7 @@
       <c r="N1408" s="21" t="s">
         <v>463</v>
       </c>
-      <c r="O1408" s="68" t="s">
+      <c r="O1408" s="62" t="s">
         <v>1</v>
       </c>
       <c r="P1408" s="24"/>
@@ -54986,7 +54977,7 @@
       <c r="N1413" s="21" t="s">
         <v>350</v>
       </c>
-      <c r="O1413" s="68" t="s">
+      <c r="O1413" s="62" t="s">
         <v>1</v>
       </c>
       <c r="P1413" s="24"/>
@@ -55144,7 +55135,7 @@
       <c r="N1417" s="21" t="s">
         <v>350</v>
       </c>
-      <c r="O1417" s="68" t="s">
+      <c r="O1417" s="62" t="s">
         <v>1</v>
       </c>
       <c r="P1417" s="24"/>
@@ -63939,7 +63930,7 @@
       <c r="N1641" s="21" t="s">
         <v>901</v>
       </c>
-      <c r="O1641" s="68" t="s">
+      <c r="O1641" s="62" t="s">
         <v>1</v>
       </c>
       <c r="P1641" s="24"/>

</xml_diff>

<commit_message>
nmv 08 03 2022
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Padam Input Templates/TS 4.7 Padam Input Template.xlsx
+++ b/TS Jatai Working/Padam Input Templates/TS 4.7 Padam Input Template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ALL IMP DATA\GitHub\texts\TS Jatai Working\Padam Input Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDC954F2-FFEA-433A-BE1E-AA0549FF83EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CAB3BD0-1EC0-4EE5-A1F7-6427C6EFD4AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4714,10 +4714,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W2010"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1636" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2004" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="H1" sqref="H1"/>
-      <selection pane="bottomLeft" activeCell="T1638" sqref="T1638"/>
+      <selection pane="bottomLeft" activeCell="N2006" sqref="N2006"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
nmv 13 03 2023
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Padam Input Templates/TS 4.7 Padam Input Template.xlsx
+++ b/TS Jatai Working/Padam Input Templates/TS 4.7 Padam Input Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ALL IMP DATA\GitHub\texts\TS Jatai Working\Padam Input Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DEA96CA-7300-4F28-96C7-B9FD94F12D67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63E45CA1-2504-4028-AA05-810412B269BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3675,9 +3675,6 @@
     <t xml:space="preserve"> neqSaqt </t>
   </si>
   <si>
-    <t xml:space="preserve"> aqBiqmAqtiqsAha$m </t>
-  </si>
-  <si>
     <t xml:space="preserve"> nyaqrtthAt </t>
   </si>
   <si>
@@ -4048,6 +4045,9 @@
   </si>
   <si>
     <t>uqttaqma ityu#t - taqmaH</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> aqBiqmAqtiqShAha$m </t>
   </si>
 </sst>
 </file>
@@ -4715,9 +4715,9 @@
   <dimension ref="A1:W2010"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="I1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1434" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A1593" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="H1" sqref="H1"/>
-      <selection pane="bottomLeft" activeCell="V1446" sqref="V1446"/>
+      <selection pane="bottomLeft" activeCell="N1607" sqref="N1607"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -5276,7 +5276,7 @@
         <v>1</v>
       </c>
       <c r="N2" s="21" t="s">
-        <v>1329</v>
+        <v>1328</v>
       </c>
       <c r="O2" s="23" t="s">
         <v>16</v>
@@ -5495,7 +5495,7 @@
       <c r="T7" s="15"/>
       <c r="U7" s="15"/>
       <c r="V7" s="5" t="s">
-        <v>1243</v>
+        <v>1242</v>
       </c>
     </row>
     <row r="8" spans="1:22" s="9" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -5526,7 +5526,7 @@
         <v>7</v>
       </c>
       <c r="N8" s="55" t="s">
-        <v>1331</v>
+        <v>1330</v>
       </c>
       <c r="O8" s="23"/>
       <c r="P8" s="23"/>
@@ -5656,7 +5656,7 @@
       <c r="T11" s="15"/>
       <c r="U11" s="15"/>
       <c r="V11" s="21" t="s">
-        <v>1244</v>
+        <v>1243</v>
       </c>
     </row>
     <row r="12" spans="1:22" s="9" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -9681,7 +9681,7 @@
       <c r="T119" s="8"/>
       <c r="U119" s="8"/>
       <c r="V119" s="5" t="s">
-        <v>1245</v>
+        <v>1244</v>
       </c>
     </row>
     <row r="120" spans="9:22" s="6" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -13481,7 +13481,7 @@
       <c r="T233" s="8"/>
       <c r="U233" s="8"/>
       <c r="V233" s="5" t="s">
-        <v>1245</v>
+        <v>1244</v>
       </c>
     </row>
     <row r="234" spans="4:22" s="6" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -13811,7 +13811,7 @@
       <c r="T243" s="8"/>
       <c r="U243" s="8"/>
       <c r="V243" s="61" t="s">
-        <v>1336</v>
+        <v>1335</v>
       </c>
     </row>
     <row r="244" spans="9:22" s="6" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -15687,7 +15687,7 @@
         <v>67</v>
       </c>
       <c r="N300" s="55" t="s">
-        <v>1332</v>
+        <v>1331</v>
       </c>
       <c r="O300" s="23"/>
       <c r="P300" s="23"/>
@@ -17060,7 +17060,7 @@
       <c r="T341" s="8"/>
       <c r="U341" s="8"/>
       <c r="V341" s="5" t="s">
-        <v>1245</v>
+        <v>1244</v>
       </c>
     </row>
     <row r="342" spans="9:22" s="6" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -20832,7 +20832,7 @@
       <c r="T455" s="8"/>
       <c r="U455" s="8"/>
       <c r="V455" s="5" t="s">
-        <v>1246</v>
+        <v>1245</v>
       </c>
     </row>
     <row r="456" spans="5:22" s="6" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -24076,7 +24076,7 @@
       <c r="T553" s="8"/>
       <c r="U553" s="8"/>
       <c r="V553" s="5" t="s">
-        <v>1246</v>
+        <v>1245</v>
       </c>
     </row>
     <row r="554" spans="9:22" s="6" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -28072,7 +28072,7 @@
       <c r="T674" s="8"/>
       <c r="U674" s="8"/>
       <c r="V674" s="5" t="s">
-        <v>1246</v>
+        <v>1245</v>
       </c>
     </row>
     <row r="675" spans="8:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -29821,7 +29821,7 @@
       <c r="T726" s="8"/>
       <c r="U726" s="8"/>
       <c r="V726" s="57" t="s">
-        <v>1333</v>
+        <v>1332</v>
       </c>
     </row>
     <row r="727" spans="9:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -30889,7 +30889,7 @@
       <c r="T758" s="8"/>
       <c r="U758" s="8"/>
       <c r="V758" s="5" t="s">
-        <v>1246</v>
+        <v>1245</v>
       </c>
     </row>
     <row r="759" spans="9:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -33087,7 +33087,7 @@
       <c r="T824" s="8"/>
       <c r="U824" s="8"/>
       <c r="V824" s="5" t="s">
-        <v>1246</v>
+        <v>1245</v>
       </c>
     </row>
     <row r="825" spans="9:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -35384,7 +35384,7 @@
       <c r="T892" s="8"/>
       <c r="U892" s="8"/>
       <c r="V892" s="36" t="s">
-        <v>1247</v>
+        <v>1246</v>
       </c>
     </row>
     <row r="893" spans="8:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -38413,7 +38413,7 @@
       <c r="T982" s="8"/>
       <c r="U982" s="8"/>
       <c r="V982" s="5" t="s">
-        <v>1248</v>
+        <v>1247</v>
       </c>
     </row>
     <row r="983" spans="9:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -39545,7 +39545,7 @@
       <c r="T1016" s="8"/>
       <c r="U1016" s="8"/>
       <c r="V1016" s="54" t="s">
-        <v>1330</v>
+        <v>1329</v>
       </c>
     </row>
     <row r="1017" spans="9:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -42158,7 +42158,7 @@
       <c r="T1093" s="8"/>
       <c r="U1093" s="8"/>
       <c r="V1093" s="5" t="s">
-        <v>1249</v>
+        <v>1248</v>
       </c>
     </row>
     <row r="1094" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -42444,7 +42444,7 @@
       <c r="T1100" s="8"/>
       <c r="U1100" s="8"/>
       <c r="V1100" s="36" t="s">
-        <v>1250</v>
+        <v>1249</v>
       </c>
     </row>
     <row r="1101" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -42721,7 +42721,7 @@
       <c r="T1107" s="8"/>
       <c r="U1107" s="8"/>
       <c r="V1107" s="5" t="s">
-        <v>1251</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="1108" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -43080,7 +43080,7 @@
       <c r="T1116" s="8"/>
       <c r="U1116" s="8"/>
       <c r="V1116" s="36" t="s">
-        <v>1252</v>
+        <v>1251</v>
       </c>
     </row>
     <row r="1117" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -43533,7 +43533,7 @@
         <v>981</v>
       </c>
       <c r="V1127" s="36" t="s">
-        <v>1253</v>
+        <v>1252</v>
       </c>
     </row>
     <row r="1128" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -43772,7 +43772,7 @@
       <c r="T1133" s="8"/>
       <c r="U1133" s="8"/>
       <c r="V1133" s="36" t="s">
-        <v>1254</v>
+        <v>1253</v>
       </c>
     </row>
     <row r="1134" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -43973,7 +43973,7 @@
       <c r="T1138" s="8"/>
       <c r="U1138" s="8"/>
       <c r="V1138" s="36" t="s">
-        <v>1255</v>
+        <v>1254</v>
       </c>
     </row>
     <row r="1139" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -44290,7 +44290,7 @@
       <c r="T1146" s="8"/>
       <c r="U1146" s="8"/>
       <c r="V1146" s="36" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
     </row>
     <row r="1147" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -44967,7 +44967,7 @@
       <c r="T1163" s="8"/>
       <c r="U1163" s="8"/>
       <c r="V1163" s="36" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
     </row>
     <row r="1164" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -45285,7 +45285,7 @@
       <c r="T1171" s="8"/>
       <c r="U1171" s="8"/>
       <c r="V1171" s="36" t="s">
-        <v>1258</v>
+        <v>1257</v>
       </c>
     </row>
     <row r="1172" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -45640,7 +45640,7 @@
       <c r="T1180" s="8"/>
       <c r="U1180" s="8"/>
       <c r="V1180" s="5" t="s">
-        <v>1259</v>
+        <v>1258</v>
       </c>
     </row>
     <row r="1181" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -45800,7 +45800,7 @@
       <c r="T1184" s="8"/>
       <c r="U1184" s="8"/>
       <c r="V1184" s="36" t="s">
-        <v>1260</v>
+        <v>1259</v>
       </c>
     </row>
     <row r="1185" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -46394,7 +46394,7 @@
         <v>898</v>
       </c>
       <c r="V1199" s="5" t="s">
-        <v>1261</v>
+        <v>1260</v>
       </c>
     </row>
     <row r="1200" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -46677,7 +46677,7 @@
       <c r="T1206" s="8"/>
       <c r="U1206" s="8"/>
       <c r="V1206" s="36" t="s">
-        <v>1262</v>
+        <v>1261</v>
       </c>
     </row>
     <row r="1207" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -47078,7 +47078,7 @@
       <c r="T1216" s="8"/>
       <c r="U1216" s="8"/>
       <c r="V1216" s="36" t="s">
-        <v>1263</v>
+        <v>1262</v>
       </c>
     </row>
     <row r="1217" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -48225,7 +48225,7 @@
       <c r="T1245" s="8"/>
       <c r="U1245" s="8"/>
       <c r="V1245" s="5" t="s">
-        <v>1264</v>
+        <v>1263</v>
       </c>
     </row>
     <row r="1246" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -48548,7 +48548,7 @@
       <c r="T1253" s="8"/>
       <c r="U1253" s="8"/>
       <c r="V1253" s="36" t="s">
-        <v>1265</v>
+        <v>1264</v>
       </c>
     </row>
     <row r="1254" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -48782,7 +48782,7 @@
         <v>909</v>
       </c>
       <c r="T1259" s="56" t="s">
-        <v>1334</v>
+        <v>1333</v>
       </c>
       <c r="U1259" s="8"/>
       <c r="V1259" s="5" t="s">
@@ -48947,7 +48947,7 @@
       <c r="T1263" s="8"/>
       <c r="U1263" s="8"/>
       <c r="V1263" s="48" t="s">
-        <v>1266</v>
+        <v>1265</v>
       </c>
     </row>
     <row r="1264" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -49323,7 +49323,7 @@
         <v>898</v>
       </c>
       <c r="V1272" s="5" t="s">
-        <v>1261</v>
+        <v>1260</v>
       </c>
     </row>
     <row r="1273" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -49719,7 +49719,7 @@
       <c r="T1282" s="8"/>
       <c r="U1282" s="8"/>
       <c r="V1282" s="5" t="s">
-        <v>1267</v>
+        <v>1266</v>
       </c>
     </row>
     <row r="1283" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -49998,7 +49998,7 @@
       <c r="T1289" s="8"/>
       <c r="U1289" s="8"/>
       <c r="V1289" s="36" t="s">
-        <v>1268</v>
+        <v>1267</v>
       </c>
     </row>
     <row r="1290" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -50317,7 +50317,7 @@
       <c r="T1297" s="8"/>
       <c r="U1297" s="8"/>
       <c r="V1297" s="36" t="s">
-        <v>1269</v>
+        <v>1268</v>
       </c>
     </row>
     <row r="1298" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -50750,7 +50750,7 @@
       <c r="T1308" s="8"/>
       <c r="U1308" s="8"/>
       <c r="V1308" s="36" t="s">
-        <v>1270</v>
+        <v>1269</v>
       </c>
     </row>
     <row r="1309" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -51074,7 +51074,7 @@
         <v>898</v>
       </c>
       <c r="V1316" s="5" t="s">
-        <v>1271</v>
+        <v>1270</v>
       </c>
     </row>
     <row r="1317" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -51546,7 +51546,7 @@
       <c r="T1328" s="8"/>
       <c r="U1328" s="8"/>
       <c r="V1328" s="36" t="s">
-        <v>1272</v>
+        <v>1271</v>
       </c>
     </row>
     <row r="1329" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -51860,7 +51860,7 @@
       <c r="T1336" s="8"/>
       <c r="U1336" s="8"/>
       <c r="V1336" s="5" t="s">
-        <v>1273</v>
+        <v>1272</v>
       </c>
     </row>
     <row r="1337" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -52065,7 +52065,7 @@
       <c r="T1341" s="8"/>
       <c r="U1341" s="8"/>
       <c r="V1341" s="5" t="s">
-        <v>1274</v>
+        <v>1273</v>
       </c>
     </row>
     <row r="1342" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -52876,7 +52876,7 @@
       <c r="T1361" s="8"/>
       <c r="U1361" s="8"/>
       <c r="V1361" s="37" t="s">
-        <v>1275</v>
+        <v>1274</v>
       </c>
     </row>
     <row r="1362" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -53270,7 +53270,7 @@
       <c r="T1371" s="8"/>
       <c r="U1371" s="8"/>
       <c r="V1371" s="63" t="s">
-        <v>1338</v>
+        <v>1337</v>
       </c>
     </row>
     <row r="1372" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -53649,7 +53649,7 @@
       <c r="T1380" s="8"/>
       <c r="U1380" s="8"/>
       <c r="V1380" s="5" t="s">
-        <v>1276</v>
+        <v>1275</v>
       </c>
     </row>
     <row r="1381" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -54004,7 +54004,7 @@
       <c r="T1389" s="8"/>
       <c r="U1389" s="8"/>
       <c r="V1389" s="5" t="s">
-        <v>1277</v>
+        <v>1276</v>
       </c>
     </row>
     <row r="1390" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -54323,7 +54323,7 @@
       <c r="T1397" s="8"/>
       <c r="U1397" s="8"/>
       <c r="V1397" s="5" t="s">
-        <v>1278</v>
+        <v>1277</v>
       </c>
     </row>
     <row r="1398" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -54616,7 +54616,7 @@
       <c r="T1404" s="8"/>
       <c r="U1404" s="8"/>
       <c r="V1404" s="36" t="s">
-        <v>1279</v>
+        <v>1278</v>
       </c>
     </row>
     <row r="1405" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -54933,7 +54933,7 @@
       <c r="T1412" s="8"/>
       <c r="U1412" s="8"/>
       <c r="V1412" s="5" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
     </row>
     <row r="1413" spans="1:23" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -55383,7 +55383,7 @@
       <c r="T1423" s="8"/>
       <c r="U1423" s="8"/>
       <c r="V1423" s="5" t="s">
-        <v>1281</v>
+        <v>1280</v>
       </c>
     </row>
     <row r="1424" spans="1:23" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -55753,7 +55753,7 @@
       <c r="T1432" s="8"/>
       <c r="U1432" s="8"/>
       <c r="V1432" s="5" t="s">
-        <v>1282</v>
+        <v>1281</v>
       </c>
     </row>
     <row r="1433" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -56329,7 +56329,7 @@
       <c r="T1446" s="8"/>
       <c r="U1446" s="8"/>
       <c r="V1446" s="63" t="s">
-        <v>1339</v>
+        <v>1338</v>
       </c>
     </row>
     <row r="1447" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -56764,7 +56764,7 @@
       <c r="T1457" s="8"/>
       <c r="U1457" s="8"/>
       <c r="V1457" s="36" t="s">
-        <v>1249</v>
+        <v>1248</v>
       </c>
     </row>
     <row r="1458" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -57122,7 +57122,7 @@
       <c r="T1466" s="8"/>
       <c r="U1466" s="8"/>
       <c r="V1466" s="5" t="s">
-        <v>1283</v>
+        <v>1282</v>
       </c>
     </row>
     <row r="1467" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -57411,7 +57411,7 @@
         <v>897</v>
       </c>
       <c r="V1473" s="5" t="s">
-        <v>1284</v>
+        <v>1283</v>
       </c>
     </row>
     <row r="1474" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -57770,7 +57770,7 @@
       <c r="T1482" s="8"/>
       <c r="U1482" s="8"/>
       <c r="V1482" s="5" t="s">
-        <v>1285</v>
+        <v>1284</v>
       </c>
     </row>
     <row r="1483" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -58179,7 +58179,7 @@
       <c r="T1492" s="8"/>
       <c r="U1492" s="8"/>
       <c r="V1492" s="5" t="s">
-        <v>1286</v>
+        <v>1285</v>
       </c>
     </row>
     <row r="1493" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -58497,7 +58497,7 @@
       <c r="T1500" s="8"/>
       <c r="U1500" s="8"/>
       <c r="V1500" s="5" t="s">
-        <v>1287</v>
+        <v>1286</v>
       </c>
     </row>
     <row r="1501" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -58854,7 +58854,7 @@
       <c r="T1509" s="8"/>
       <c r="U1509" s="8"/>
       <c r="V1509" s="5" t="s">
-        <v>1288</v>
+        <v>1287</v>
       </c>
     </row>
     <row r="1510" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -59270,7 +59270,7 @@
         <v>897</v>
       </c>
       <c r="V1519" s="5" t="s">
-        <v>1289</v>
+        <v>1288</v>
       </c>
     </row>
     <row r="1520" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -59981,7 +59981,7 @@
       <c r="T1537" s="8"/>
       <c r="U1537" s="8"/>
       <c r="V1537" s="36" t="s">
-        <v>1290</v>
+        <v>1289</v>
       </c>
     </row>
     <row r="1538" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -60377,7 +60377,7 @@
         <v>897</v>
       </c>
       <c r="V1547" s="36" t="s">
-        <v>1291</v>
+        <v>1290</v>
       </c>
     </row>
     <row r="1548" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -60881,7 +60881,7 @@
       <c r="T1559" s="8"/>
       <c r="U1559" s="8"/>
       <c r="V1559" s="5" t="s">
-        <v>1246</v>
+        <v>1245</v>
       </c>
     </row>
     <row r="1560" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -61255,7 +61255,7 @@
       <c r="T1568" s="8"/>
       <c r="U1568" s="8"/>
       <c r="V1568" s="36" t="s">
-        <v>1292</v>
+        <v>1291</v>
       </c>
     </row>
     <row r="1569" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -61649,7 +61649,7 @@
       <c r="T1578" s="8"/>
       <c r="U1578" s="8"/>
       <c r="V1578" s="48" t="s">
-        <v>1293</v>
+        <v>1292</v>
       </c>
     </row>
     <row r="1579" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -62007,7 +62007,7 @@
         <v>18</v>
       </c>
       <c r="V1588" s="36" t="s">
-        <v>1294</v>
+        <v>1293</v>
       </c>
     </row>
     <row r="1589" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -62417,7 +62417,7 @@
         <v>18</v>
       </c>
       <c r="V1599" s="5" t="s">
-        <v>1295</v>
+        <v>1294</v>
       </c>
     </row>
     <row r="1600" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -62707,8 +62707,8 @@
         <f t="shared" ref="M1607" si="166">+M1606+1</f>
         <v>125</v>
       </c>
-      <c r="N1607" s="21" t="s">
-        <v>1215</v>
+      <c r="N1607" s="16" t="s">
+        <v>1339</v>
       </c>
       <c r="O1607" s="23" t="s">
         <v>0</v>
@@ -62717,7 +62717,7 @@
         <v>18</v>
       </c>
       <c r="V1607" s="36" t="s">
-        <v>1296</v>
+        <v>1295</v>
       </c>
     </row>
     <row r="1608" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -63030,7 +63030,7 @@
         <v>134</v>
       </c>
       <c r="N1616" s="21" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
       <c r="O1616" s="23" t="s">
         <v>0</v>
@@ -63039,7 +63039,7 @@
         <v>18</v>
       </c>
       <c r="V1616" s="36" t="s">
-        <v>1297</v>
+        <v>1296</v>
       </c>
     </row>
     <row r="1617" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -63362,14 +63362,14 @@
         <v>143</v>
       </c>
       <c r="N1625" s="21" t="s">
-        <v>1217</v>
+        <v>1216</v>
       </c>
       <c r="O1625" s="23"/>
       <c r="P1625" s="24" t="s">
         <v>18</v>
       </c>
       <c r="V1625" s="5" t="s">
-        <v>1298</v>
+        <v>1297</v>
       </c>
     </row>
     <row r="1626" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -63777,14 +63777,14 @@
         <v>155</v>
       </c>
       <c r="N1637" s="21" t="s">
-        <v>1218</v>
+        <v>1217</v>
       </c>
       <c r="O1637" s="23"/>
       <c r="P1637" s="24" t="s">
         <v>18</v>
       </c>
       <c r="V1637" s="63" t="s">
-        <v>1337</v>
+        <v>1336</v>
       </c>
     </row>
     <row r="1638" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -64135,7 +64135,7 @@
         <v>165</v>
       </c>
       <c r="N1647" s="21" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
       <c r="O1647" s="23"/>
       <c r="P1647" s="24" t="s">
@@ -64148,7 +64148,7 @@
         <v>1121</v>
       </c>
       <c r="V1647" s="5" t="s">
-        <v>1299</v>
+        <v>1298</v>
       </c>
     </row>
     <row r="1648" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -64465,14 +64465,14 @@
         <v>174</v>
       </c>
       <c r="N1656" s="21" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="O1656" s="23"/>
       <c r="P1656" s="24" t="s">
         <v>18</v>
       </c>
       <c r="V1656" s="5" t="s">
-        <v>1300</v>
+        <v>1299</v>
       </c>
     </row>
     <row r="1657" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -64792,7 +64792,7 @@
         <v>18</v>
       </c>
       <c r="V1665" s="36" t="s">
-        <v>1301</v>
+        <v>1300</v>
       </c>
     </row>
     <row r="1666" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -65134,14 +65134,14 @@
         <v>193</v>
       </c>
       <c r="N1675" s="21" t="s">
-        <v>1221</v>
+        <v>1220</v>
       </c>
       <c r="O1675" s="23"/>
       <c r="P1675" s="24" t="s">
         <v>18</v>
       </c>
       <c r="V1675" s="36" t="s">
-        <v>1302</v>
+        <v>1301</v>
       </c>
     </row>
     <row r="1676" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -65398,7 +65398,7 @@
         <v>8</v>
       </c>
       <c r="N1683" s="21" t="s">
-        <v>1222</v>
+        <v>1221</v>
       </c>
       <c r="O1683" s="23" t="s">
         <v>0</v>
@@ -65407,7 +65407,7 @@
         <v>18</v>
       </c>
       <c r="V1683" s="36" t="s">
-        <v>1303</v>
+        <v>1302</v>
       </c>
     </row>
     <row r="1684" spans="3:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -65664,7 +65664,7 @@
         <v>16</v>
       </c>
       <c r="N1691" s="46" t="s">
-        <v>1223</v>
+        <v>1222</v>
       </c>
       <c r="O1691" s="23"/>
       <c r="P1691" s="24" t="s">
@@ -65674,7 +65674,7 @@
         <v>898</v>
       </c>
       <c r="V1691" s="36" t="s">
-        <v>1304</v>
+        <v>1303</v>
       </c>
     </row>
     <row r="1692" spans="3:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -66032,14 +66032,14 @@
         <v>27</v>
       </c>
       <c r="N1702" s="21" t="s">
-        <v>1224</v>
+        <v>1223</v>
       </c>
       <c r="O1702" s="23"/>
       <c r="P1702" s="24" t="s">
         <v>18</v>
       </c>
       <c r="V1702" s="36" t="s">
-        <v>1305</v>
+        <v>1304</v>
       </c>
     </row>
     <row r="1703" spans="3:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -66285,7 +66285,7 @@
         <v>35</v>
       </c>
       <c r="N1710" s="21" t="s">
-        <v>1223</v>
+        <v>1222</v>
       </c>
       <c r="O1710" s="23"/>
       <c r="P1710" s="24" t="s">
@@ -66295,7 +66295,7 @@
         <v>898</v>
       </c>
       <c r="V1710" s="5" t="s">
-        <v>1304</v>
+        <v>1303</v>
       </c>
     </row>
     <row r="1711" spans="3:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -66573,7 +66573,7 @@
         <v>44</v>
       </c>
       <c r="N1719" s="21" t="s">
-        <v>1225</v>
+        <v>1224</v>
       </c>
       <c r="O1719" s="23" t="s">
         <v>0</v>
@@ -66888,7 +66888,7 @@
         <v>54</v>
       </c>
       <c r="N1729" s="21" t="s">
-        <v>1223</v>
+        <v>1222</v>
       </c>
       <c r="O1729" s="23"/>
       <c r="P1729" s="24" t="s">
@@ -66898,7 +66898,7 @@
         <v>898</v>
       </c>
       <c r="V1729" s="5" t="s">
-        <v>1304</v>
+        <v>1303</v>
       </c>
     </row>
     <row r="1730" spans="3:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -67207,14 +67207,14 @@
         <v>64</v>
       </c>
       <c r="N1739" s="21" t="s">
-        <v>1226</v>
+        <v>1225</v>
       </c>
       <c r="O1739" s="23"/>
       <c r="P1739" s="24" t="s">
         <v>18</v>
       </c>
       <c r="V1739" s="36" t="s">
-        <v>1306</v>
+        <v>1305</v>
       </c>
     </row>
     <row r="1740" spans="3:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -67457,7 +67457,7 @@
         <v>72</v>
       </c>
       <c r="N1747" s="21" t="s">
-        <v>1223</v>
+        <v>1222</v>
       </c>
       <c r="O1747" s="23"/>
       <c r="P1747" s="24" t="s">
@@ -67467,7 +67467,7 @@
         <v>898</v>
       </c>
       <c r="V1747" s="5" t="s">
-        <v>1304</v>
+        <v>1303</v>
       </c>
     </row>
     <row r="1748" spans="3:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -67754,7 +67754,7 @@
         <v>18</v>
       </c>
       <c r="V1756" s="36" t="s">
-        <v>1307</v>
+        <v>1306</v>
       </c>
     </row>
     <row r="1757" spans="3:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -68030,14 +68030,14 @@
         <v>90</v>
       </c>
       <c r="N1765" s="21" t="s">
-        <v>1227</v>
+        <v>1226</v>
       </c>
       <c r="O1765" s="23"/>
       <c r="P1765" s="24" t="s">
         <v>18</v>
       </c>
       <c r="V1765" s="36" t="s">
-        <v>1308</v>
+        <v>1307</v>
       </c>
     </row>
     <row r="1766" spans="3:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -68341,14 +68341,14 @@
         <v>99</v>
       </c>
       <c r="N1774" s="21" t="s">
-        <v>1228</v>
+        <v>1227</v>
       </c>
       <c r="O1774" s="23"/>
       <c r="P1774" s="24" t="s">
         <v>18</v>
       </c>
       <c r="V1774" s="36" t="s">
-        <v>1309</v>
+        <v>1308</v>
       </c>
     </row>
     <row r="1775" spans="3:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -68592,14 +68592,14 @@
         <v>107</v>
       </c>
       <c r="N1782" s="21" t="s">
-        <v>1227</v>
+        <v>1226</v>
       </c>
       <c r="O1782" s="23"/>
       <c r="P1782" s="24" t="s">
         <v>18</v>
       </c>
       <c r="V1782" s="5" t="s">
-        <v>1308</v>
+        <v>1307</v>
       </c>
     </row>
     <row r="1783" spans="3:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -68912,14 +68912,14 @@
         <v>117</v>
       </c>
       <c r="N1792" s="21" t="s">
-        <v>1229</v>
+        <v>1228</v>
       </c>
       <c r="O1792" s="23"/>
       <c r="P1792" s="24" t="s">
         <v>18</v>
       </c>
       <c r="V1792" s="5" t="s">
-        <v>1310</v>
+        <v>1309</v>
       </c>
     </row>
     <row r="1793" spans="3:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -69164,14 +69164,14 @@
         <v>125</v>
       </c>
       <c r="N1800" s="21" t="s">
-        <v>1227</v>
+        <v>1226</v>
       </c>
       <c r="O1800" s="23"/>
       <c r="P1800" s="24" t="s">
         <v>18</v>
       </c>
       <c r="V1800" s="5" t="s">
-        <v>1308</v>
+        <v>1307</v>
       </c>
     </row>
     <row r="1801" spans="3:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -69385,7 +69385,7 @@
         <v>132</v>
       </c>
       <c r="N1807" s="21" t="s">
-        <v>1230</v>
+        <v>1229</v>
       </c>
       <c r="O1807" s="23"/>
       <c r="P1807" s="24" t="s">
@@ -69395,7 +69395,7 @@
         <v>897</v>
       </c>
       <c r="V1807" s="5" t="s">
-        <v>1311</v>
+        <v>1310</v>
       </c>
     </row>
     <row r="1808" spans="3:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -69669,14 +69669,14 @@
         <v>141</v>
       </c>
       <c r="N1816" s="21" t="s">
-        <v>1227</v>
+        <v>1226</v>
       </c>
       <c r="O1816" s="23"/>
       <c r="P1816" s="24" t="s">
         <v>18</v>
       </c>
       <c r="V1816" s="5" t="s">
-        <v>1308</v>
+        <v>1307</v>
       </c>
     </row>
     <row r="1817" spans="3:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -69926,14 +69926,14 @@
         <v>149</v>
       </c>
       <c r="N1824" s="21" t="s">
-        <v>1231</v>
+        <v>1230</v>
       </c>
       <c r="O1824" s="23"/>
       <c r="P1824" s="24" t="s">
         <v>18</v>
       </c>
       <c r="V1824" s="5" t="s">
-        <v>1312</v>
+        <v>1311</v>
       </c>
     </row>
     <row r="1825" spans="3:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -70245,14 +70245,14 @@
         <v>159</v>
       </c>
       <c r="N1834" s="21" t="s">
-        <v>1227</v>
+        <v>1226</v>
       </c>
       <c r="O1834" s="23"/>
       <c r="P1834" s="24" t="s">
         <v>18</v>
       </c>
       <c r="V1834" s="5" t="s">
-        <v>1308</v>
+        <v>1307</v>
       </c>
     </row>
     <row r="1835" spans="3:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -70468,14 +70468,14 @@
         <v>166</v>
       </c>
       <c r="N1841" s="21" t="s">
-        <v>1232</v>
+        <v>1231</v>
       </c>
       <c r="O1841" s="23"/>
       <c r="P1841" s="24" t="s">
         <v>18</v>
       </c>
       <c r="V1841" s="5" t="s">
-        <v>1313</v>
+        <v>1312</v>
       </c>
     </row>
     <row r="1842" spans="3:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -70752,14 +70752,14 @@
         <v>175</v>
       </c>
       <c r="N1850" s="21" t="s">
-        <v>1227</v>
+        <v>1226</v>
       </c>
       <c r="O1850" s="23"/>
       <c r="P1850" s="24" t="s">
         <v>18</v>
       </c>
       <c r="V1850" s="5" t="s">
-        <v>1308</v>
+        <v>1307</v>
       </c>
     </row>
     <row r="1851" spans="3:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -71110,14 +71110,14 @@
         <v>186</v>
       </c>
       <c r="N1861" s="21" t="s">
-        <v>1233</v>
+        <v>1232</v>
       </c>
       <c r="O1861" s="23"/>
       <c r="P1861" s="24" t="s">
         <v>18</v>
       </c>
       <c r="V1861" s="36" t="s">
-        <v>1314</v>
+        <v>1313</v>
       </c>
     </row>
     <row r="1862" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -71362,14 +71362,14 @@
         <v>194</v>
       </c>
       <c r="N1869" s="21" t="s">
-        <v>1234</v>
+        <v>1233</v>
       </c>
       <c r="O1869" s="23"/>
       <c r="P1869" s="24" t="s">
         <v>18</v>
       </c>
       <c r="V1869" s="5" t="s">
-        <v>1315</v>
+        <v>1314</v>
       </c>
     </row>
     <row r="1870" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -71611,14 +71611,14 @@
         <v>202</v>
       </c>
       <c r="N1877" s="21" t="s">
-        <v>1235</v>
+        <v>1234</v>
       </c>
       <c r="O1877" s="23"/>
       <c r="P1877" s="24" t="s">
         <v>18</v>
       </c>
       <c r="V1877" s="5" t="s">
-        <v>1316</v>
+        <v>1315</v>
       </c>
     </row>
     <row r="1878" spans="3:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -71892,14 +71892,14 @@
         <v>211</v>
       </c>
       <c r="N1886" s="21" t="s">
-        <v>1234</v>
+        <v>1233</v>
       </c>
       <c r="O1886" s="23"/>
       <c r="P1886" s="24" t="s">
         <v>18</v>
       </c>
       <c r="V1886" s="5" t="s">
-        <v>1315</v>
+        <v>1314</v>
       </c>
     </row>
     <row r="1887" spans="3:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -72238,14 +72238,14 @@
         <v>222</v>
       </c>
       <c r="N1897" s="21" t="s">
-        <v>1233</v>
+        <v>1232</v>
       </c>
       <c r="O1897" s="23"/>
       <c r="P1897" s="24" t="s">
         <v>18</v>
       </c>
       <c r="V1897" s="5" t="s">
-        <v>1314</v>
+        <v>1313</v>
       </c>
     </row>
     <row r="1898" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -72493,14 +72493,14 @@
         <v>230</v>
       </c>
       <c r="N1905" s="21" t="s">
-        <v>1234</v>
+        <v>1233</v>
       </c>
       <c r="O1905" s="23"/>
       <c r="P1905" s="24" t="s">
         <v>18</v>
       </c>
       <c r="V1905" s="36" t="s">
-        <v>1315</v>
+        <v>1314</v>
       </c>
     </row>
     <row r="1906" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -72698,14 +72698,14 @@
         <v>236</v>
       </c>
       <c r="N1911" s="21" t="s">
-        <v>1236</v>
+        <v>1235</v>
       </c>
       <c r="O1911" s="23"/>
       <c r="P1911" s="24" t="s">
         <v>18</v>
       </c>
       <c r="V1911" s="36" t="s">
-        <v>1317</v>
+        <v>1316</v>
       </c>
     </row>
     <row r="1912" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -72982,14 +72982,14 @@
         <v>245</v>
       </c>
       <c r="N1920" s="21" t="s">
-        <v>1234</v>
+        <v>1233</v>
       </c>
       <c r="O1920" s="23"/>
       <c r="P1920" s="24" t="s">
         <v>18</v>
       </c>
       <c r="V1920" s="5" t="s">
-        <v>1315</v>
+        <v>1314</v>
       </c>
     </row>
     <row r="1921" spans="3:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -73417,14 +73417,14 @@
         <v>258</v>
       </c>
       <c r="N1933" s="21" t="s">
-        <v>1237</v>
+        <v>1236</v>
       </c>
       <c r="O1933" s="23"/>
       <c r="P1933" s="24" t="s">
         <v>18</v>
       </c>
       <c r="V1933" s="5" t="s">
-        <v>1318</v>
+        <v>1317</v>
       </c>
     </row>
     <row r="1934" spans="3:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -73457,7 +73457,7 @@
       </c>
       <c r="P1934" s="24"/>
       <c r="V1934" s="36" t="s">
-        <v>1319</v>
+        <v>1318</v>
       </c>
     </row>
     <row r="1935" spans="3:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -73681,14 +73681,14 @@
         <v>266</v>
       </c>
       <c r="N1941" s="21" t="s">
-        <v>1238</v>
+        <v>1237</v>
       </c>
       <c r="O1941" s="23"/>
       <c r="P1941" s="24" t="s">
         <v>18</v>
       </c>
       <c r="V1941" s="36" t="s">
-        <v>1320</v>
+        <v>1319</v>
       </c>
     </row>
     <row r="1942" spans="3:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -73847,7 +73847,7 @@
       </c>
       <c r="P1946" s="24"/>
       <c r="V1946" s="36" t="s">
-        <v>1321</v>
+        <v>1320</v>
       </c>
     </row>
     <row r="1947" spans="3:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -73935,7 +73935,7 @@
         <v>274</v>
       </c>
       <c r="N1949" s="21" t="s">
-        <v>1223</v>
+        <v>1222</v>
       </c>
       <c r="O1949" s="23"/>
       <c r="P1949" s="24" t="s">
@@ -73945,7 +73945,7 @@
         <v>898</v>
       </c>
       <c r="V1949" s="36" t="s">
-        <v>1304</v>
+        <v>1303</v>
       </c>
     </row>
     <row r="1950" spans="3:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -73978,7 +73978,7 @@
       </c>
       <c r="P1950" s="24"/>
       <c r="V1950" s="36" t="s">
-        <v>1322</v>
+        <v>1321</v>
       </c>
     </row>
     <row r="1951" spans="3:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -74011,7 +74011,7 @@
       </c>
       <c r="P1951" s="24"/>
       <c r="V1951" s="36" t="s">
-        <v>1323</v>
+        <v>1322</v>
       </c>
     </row>
     <row r="1952" spans="3:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -74137,7 +74137,7 @@
       </c>
       <c r="P1955" s="24"/>
       <c r="V1955" s="36" t="s">
-        <v>1324</v>
+        <v>1323</v>
       </c>
     </row>
     <row r="1956" spans="3:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -74226,14 +74226,14 @@
         <v>283</v>
       </c>
       <c r="N1958" s="21" t="s">
-        <v>1239</v>
+        <v>1238</v>
       </c>
       <c r="O1958" s="23"/>
       <c r="P1958" s="24" t="s">
         <v>18</v>
       </c>
       <c r="V1958" s="5" t="s">
-        <v>1325</v>
+        <v>1324</v>
       </c>
     </row>
     <row r="1959" spans="3:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -74480,7 +74480,7 @@
         <v>291</v>
       </c>
       <c r="N1966" s="21" t="s">
-        <v>1223</v>
+        <v>1222</v>
       </c>
       <c r="O1966" s="23"/>
       <c r="P1966" s="24" t="s">
@@ -74490,7 +74490,7 @@
         <v>898</v>
       </c>
       <c r="V1966" s="5" t="s">
-        <v>1304</v>
+        <v>1303</v>
       </c>
     </row>
     <row r="1967" spans="3:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -74820,14 +74820,14 @@
         <v>301</v>
       </c>
       <c r="N1976" s="21" t="s">
-        <v>1240</v>
+        <v>1239</v>
       </c>
       <c r="O1976" s="23"/>
       <c r="P1976" s="24" t="s">
         <v>18</v>
       </c>
       <c r="V1976" s="5" t="s">
-        <v>1326</v>
+        <v>1325</v>
       </c>
     </row>
     <row r="1977" spans="3:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -74893,7 +74893,7 @@
         <v>303</v>
       </c>
       <c r="N1978" s="55" t="s">
-        <v>1335</v>
+        <v>1334</v>
       </c>
       <c r="O1978" s="23" t="s">
         <v>1</v>
@@ -75178,7 +75178,7 @@
         <v>898</v>
       </c>
       <c r="V1986" s="5" t="s">
-        <v>1261</v>
+        <v>1260</v>
       </c>
     </row>
     <row r="1987" spans="3:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -75492,14 +75492,14 @@
         <v>321</v>
       </c>
       <c r="N1996" s="21" t="s">
-        <v>1241</v>
+        <v>1240</v>
       </c>
       <c r="O1996" s="23"/>
       <c r="P1996" s="24" t="s">
         <v>18</v>
       </c>
       <c r="V1996" s="5" t="s">
-        <v>1327</v>
+        <v>1326</v>
       </c>
     </row>
     <row r="1997" spans="3:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -75917,14 +75917,14 @@
         <v>334</v>
       </c>
       <c r="N2009" s="21" t="s">
-        <v>1242</v>
+        <v>1241</v>
       </c>
       <c r="O2009" s="23"/>
       <c r="P2009" s="24" t="s">
         <v>18</v>
       </c>
       <c r="V2009" s="36" t="s">
-        <v>1328</v>
+        <v>1327</v>
       </c>
     </row>
     <row r="2010" spans="3:22" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
nmv 14 03 2023
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Padam Input Templates/TS 4.7 Padam Input Template.xlsx
+++ b/TS Jatai Working/Padam Input Templates/TS 4.7 Padam Input Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ALL IMP DATA\GitHub\texts\TS Jatai Working\Padam Input Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63E45CA1-2504-4028-AA05-810412B269BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AB403E9-88F6-49DF-8C16-E68D88820B21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8208" uniqueCount="1340">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8210" uniqueCount="1340">
   <si>
     <t>PS</t>
   </si>
@@ -4715,9 +4715,9 @@
   <dimension ref="A1:W2010"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="I1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1593" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A1989" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="H1" sqref="H1"/>
-      <selection pane="bottomLeft" activeCell="N1607" sqref="N1607"/>
+      <selection pane="bottomLeft" activeCell="V2003" sqref="V2003"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -63921,6 +63921,9 @@
         <v>1</v>
       </c>
       <c r="P1641" s="24"/>
+      <c r="U1641" s="1" t="s">
+        <v>899</v>
+      </c>
       <c r="V1641" s="5" t="s">
         <v>727</v>
       </c>
@@ -75792,6 +75795,9 @@
       </c>
       <c r="O2005" s="23"/>
       <c r="P2005" s="24"/>
+      <c r="U2005" s="1" t="s">
+        <v>899</v>
+      </c>
       <c r="V2005" s="5" t="s">
         <v>727</v>
       </c>

</xml_diff>

<commit_message>
nmv 14 05 2024
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Padam Input Templates/TS 4.7 Padam Input Template.xlsx
+++ b/TS Jatai Working/Padam Input Templates/TS 4.7 Padam Input Template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ALL IMP DATA\GitHub\texts\TS Jatai Working\Padam Input Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F448538-2D1E-400A-A05C-8FC8AA0BA08B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8273619-2DA4-451D-A329-CF3B1542D161}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3828,9 +3828,6 @@
     <t xml:space="preserve">oSha#dhInAqmityoSha#dhInAm </t>
   </si>
   <si>
-    <t xml:space="preserve">paqtha iti# pathe </t>
-  </si>
-  <si>
     <t xml:space="preserve">stIqrNaba#r.hiShaqmiti# stIqrNa - baqr.qhiqShaqm </t>
   </si>
   <si>
@@ -3933,9 +3930,6 @@
     <t xml:space="preserve">Aga#saq ityAga#saH </t>
   </si>
   <si>
-    <t xml:space="preserve">dUqShayanniti# dUqShayann# </t>
-  </si>
-  <si>
     <t xml:space="preserve">rakSha#taq itiq rakSha#taH </t>
   </si>
   <si>
@@ -4048,6 +4042,12 @@
   </si>
   <si>
     <t>nihi#taq itiq ni - hiqtaqH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">paqtha iti# paqthe </t>
+  </si>
+  <si>
+    <t xml:space="preserve">dUqShayaqnniti# dUqShayann# </t>
   </si>
 </sst>
 </file>
@@ -4425,13 +4425,13 @@
     <xf numFmtId="0" fontId="17" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4715,9 +4715,9 @@
   <dimension ref="A1:W2010"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="I1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1949" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A1762" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="H1" sqref="H1"/>
-      <selection pane="bottomLeft" activeCell="V2009" sqref="V2009"/>
+      <selection pane="bottomLeft" activeCell="N1774" sqref="N1774"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -5276,7 +5276,7 @@
         <v>1</v>
       </c>
       <c r="N2" s="21" t="s">
-        <v>1321</v>
+        <v>1319</v>
       </c>
       <c r="O2" s="23" t="s">
         <v>16</v>
@@ -5287,7 +5287,7 @@
       <c r="S2" s="15"/>
       <c r="T2" s="15"/>
       <c r="U2" s="15"/>
-      <c r="V2" s="63" t="s">
+      <c r="V2" s="62" t="s">
         <v>921</v>
       </c>
     </row>
@@ -5526,7 +5526,7 @@
         <v>7</v>
       </c>
       <c r="N8" s="55" t="s">
-        <v>1323</v>
+        <v>1321</v>
       </c>
       <c r="O8" s="23"/>
       <c r="P8" s="23"/>
@@ -13810,8 +13810,8 @@
       <c r="S243" s="8"/>
       <c r="T243" s="8"/>
       <c r="U243" s="8"/>
-      <c r="V243" s="61" t="s">
-        <v>1328</v>
+      <c r="V243" s="63" t="s">
+        <v>1326</v>
       </c>
     </row>
     <row r="244" spans="9:22" s="6" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -15687,7 +15687,7 @@
         <v>67</v>
       </c>
       <c r="N300" s="55" t="s">
-        <v>1324</v>
+        <v>1322</v>
       </c>
       <c r="O300" s="23"/>
       <c r="P300" s="23"/>
@@ -29821,7 +29821,7 @@
       <c r="T726" s="8"/>
       <c r="U726" s="8"/>
       <c r="V726" s="57" t="s">
-        <v>1325</v>
+        <v>1323</v>
       </c>
     </row>
     <row r="727" spans="9:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -29921,8 +29921,8 @@
       <c r="S729" s="8"/>
       <c r="T729" s="8"/>
       <c r="U729" s="8"/>
-      <c r="V729" s="63" t="s">
-        <v>1334</v>
+      <c r="V729" s="62" t="s">
+        <v>1332</v>
       </c>
     </row>
     <row r="730" spans="9:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -32218,8 +32218,8 @@
       <c r="S798" s="8"/>
       <c r="T798" s="8"/>
       <c r="U798" s="8"/>
-      <c r="V798" s="63" t="s">
-        <v>1335</v>
+      <c r="V798" s="62" t="s">
+        <v>1333</v>
       </c>
     </row>
     <row r="799" spans="9:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -36233,8 +36233,8 @@
       <c r="S917" s="8"/>
       <c r="T917" s="8"/>
       <c r="U917" s="8"/>
-      <c r="V917" s="63" t="s">
-        <v>1333</v>
+      <c r="V917" s="62" t="s">
+        <v>1331</v>
       </c>
     </row>
     <row r="918" spans="9:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -39545,7 +39545,7 @@
       <c r="T1016" s="8"/>
       <c r="U1016" s="8"/>
       <c r="V1016" s="54" t="s">
-        <v>1322</v>
+        <v>1320</v>
       </c>
     </row>
     <row r="1017" spans="9:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -41501,8 +41501,8 @@
       <c r="U1074" s="8" t="s">
         <v>898</v>
       </c>
-      <c r="V1074" s="63" t="s">
-        <v>1336</v>
+      <c r="V1074" s="62" t="s">
+        <v>1334</v>
       </c>
     </row>
     <row r="1075" spans="5:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -48782,7 +48782,7 @@
         <v>909</v>
       </c>
       <c r="T1259" s="56" t="s">
-        <v>1326</v>
+        <v>1324</v>
       </c>
       <c r="U1259" s="8"/>
       <c r="V1259" s="5" t="s">
@@ -52064,8 +52064,8 @@
       <c r="S1341" s="8"/>
       <c r="T1341" s="8"/>
       <c r="U1341" s="8"/>
-      <c r="V1341" s="5" t="s">
-        <v>1266</v>
+      <c r="V1341" s="62" t="s">
+        <v>1338</v>
       </c>
     </row>
     <row r="1342" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -52422,8 +52422,8 @@
       <c r="S1350" s="8"/>
       <c r="T1350" s="8"/>
       <c r="U1350" s="8"/>
-      <c r="V1350" s="63" t="s">
-        <v>1338</v>
+      <c r="V1350" s="62" t="s">
+        <v>1336</v>
       </c>
     </row>
     <row r="1351" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -52876,7 +52876,7 @@
       <c r="T1361" s="8"/>
       <c r="U1361" s="8"/>
       <c r="V1361" s="37" t="s">
-        <v>1267</v>
+        <v>1266</v>
       </c>
     </row>
     <row r="1362" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -53269,8 +53269,8 @@
       <c r="S1371" s="8"/>
       <c r="T1371" s="8"/>
       <c r="U1371" s="8"/>
-      <c r="V1371" s="63" t="s">
-        <v>1330</v>
+      <c r="V1371" s="62" t="s">
+        <v>1328</v>
       </c>
     </row>
     <row r="1372" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -53649,7 +53649,7 @@
       <c r="T1380" s="8"/>
       <c r="U1380" s="8"/>
       <c r="V1380" s="5" t="s">
-        <v>1268</v>
+        <v>1267</v>
       </c>
     </row>
     <row r="1381" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -54004,7 +54004,7 @@
       <c r="T1389" s="8"/>
       <c r="U1389" s="8"/>
       <c r="V1389" s="5" t="s">
-        <v>1269</v>
+        <v>1268</v>
       </c>
     </row>
     <row r="1390" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -54122,8 +54122,8 @@
       <c r="S1392" s="8"/>
       <c r="T1392" s="8"/>
       <c r="U1392" s="8"/>
-      <c r="V1392" s="63" t="s">
-        <v>1339</v>
+      <c r="V1392" s="62" t="s">
+        <v>1337</v>
       </c>
     </row>
     <row r="1393" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -54323,7 +54323,7 @@
       <c r="T1397" s="8"/>
       <c r="U1397" s="8"/>
       <c r="V1397" s="5" t="s">
-        <v>1270</v>
+        <v>1269</v>
       </c>
     </row>
     <row r="1398" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -54616,7 +54616,7 @@
       <c r="T1404" s="8"/>
       <c r="U1404" s="8"/>
       <c r="V1404" s="36" t="s">
-        <v>1271</v>
+        <v>1270</v>
       </c>
     </row>
     <row r="1405" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -54766,7 +54766,7 @@
       <c r="N1408" s="21" t="s">
         <v>463</v>
       </c>
-      <c r="O1408" s="62" t="s">
+      <c r="O1408" s="61" t="s">
         <v>1</v>
       </c>
       <c r="P1408" s="24"/>
@@ -54933,7 +54933,7 @@
       <c r="T1412" s="8"/>
       <c r="U1412" s="8"/>
       <c r="V1412" s="5" t="s">
-        <v>1272</v>
+        <v>1271</v>
       </c>
     </row>
     <row r="1413" spans="1:23" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -54964,7 +54964,7 @@
       <c r="N1413" s="21" t="s">
         <v>350</v>
       </c>
-      <c r="O1413" s="62" t="s">
+      <c r="O1413" s="61" t="s">
         <v>1</v>
       </c>
       <c r="P1413" s="24"/>
@@ -55122,7 +55122,7 @@
       <c r="N1417" s="21" t="s">
         <v>350</v>
       </c>
-      <c r="O1417" s="62" t="s">
+      <c r="O1417" s="61" t="s">
         <v>1</v>
       </c>
       <c r="P1417" s="24"/>
@@ -55383,7 +55383,7 @@
       <c r="T1423" s="8"/>
       <c r="U1423" s="8"/>
       <c r="V1423" s="5" t="s">
-        <v>1273</v>
+        <v>1272</v>
       </c>
     </row>
     <row r="1424" spans="1:23" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -55753,7 +55753,7 @@
       <c r="T1432" s="8"/>
       <c r="U1432" s="8"/>
       <c r="V1432" s="5" t="s">
-        <v>1274</v>
+        <v>1273</v>
       </c>
     </row>
     <row r="1433" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -56328,8 +56328,8 @@
       <c r="S1446" s="8"/>
       <c r="T1446" s="8"/>
       <c r="U1446" s="8"/>
-      <c r="V1446" s="63" t="s">
-        <v>1331</v>
+      <c r="V1446" s="62" t="s">
+        <v>1329</v>
       </c>
     </row>
     <row r="1447" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -57122,7 +57122,7 @@
       <c r="T1466" s="8"/>
       <c r="U1466" s="8"/>
       <c r="V1466" s="5" t="s">
-        <v>1275</v>
+        <v>1274</v>
       </c>
     </row>
     <row r="1467" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -57411,7 +57411,7 @@
         <v>897</v>
       </c>
       <c r="V1473" s="5" t="s">
-        <v>1276</v>
+        <v>1275</v>
       </c>
     </row>
     <row r="1474" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -57770,7 +57770,7 @@
       <c r="T1482" s="8"/>
       <c r="U1482" s="8"/>
       <c r="V1482" s="5" t="s">
-        <v>1277</v>
+        <v>1276</v>
       </c>
     </row>
     <row r="1483" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -58179,7 +58179,7 @@
       <c r="T1492" s="8"/>
       <c r="U1492" s="8"/>
       <c r="V1492" s="5" t="s">
-        <v>1278</v>
+        <v>1277</v>
       </c>
     </row>
     <row r="1493" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -58497,7 +58497,7 @@
       <c r="T1500" s="8"/>
       <c r="U1500" s="8"/>
       <c r="V1500" s="5" t="s">
-        <v>1279</v>
+        <v>1278</v>
       </c>
     </row>
     <row r="1501" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -58734,8 +58734,8 @@
       <c r="S1506" s="8"/>
       <c r="T1506" s="8"/>
       <c r="U1506" s="8"/>
-      <c r="V1506" s="63" t="s">
-        <v>1337</v>
+      <c r="V1506" s="62" t="s">
+        <v>1335</v>
       </c>
     </row>
     <row r="1507" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -58854,7 +58854,7 @@
       <c r="T1509" s="8"/>
       <c r="U1509" s="8"/>
       <c r="V1509" s="5" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
     </row>
     <row r="1510" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -59270,7 +59270,7 @@
         <v>897</v>
       </c>
       <c r="V1519" s="5" t="s">
-        <v>1281</v>
+        <v>1280</v>
       </c>
     </row>
     <row r="1520" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -59981,7 +59981,7 @@
       <c r="T1537" s="8"/>
       <c r="U1537" s="8"/>
       <c r="V1537" s="36" t="s">
-        <v>1282</v>
+        <v>1281</v>
       </c>
     </row>
     <row r="1538" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -60377,7 +60377,7 @@
         <v>897</v>
       </c>
       <c r="V1547" s="36" t="s">
-        <v>1283</v>
+        <v>1282</v>
       </c>
     </row>
     <row r="1548" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -61255,7 +61255,7 @@
       <c r="T1568" s="8"/>
       <c r="U1568" s="8"/>
       <c r="V1568" s="36" t="s">
-        <v>1284</v>
+        <v>1283</v>
       </c>
     </row>
     <row r="1569" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -61649,7 +61649,7 @@
       <c r="T1578" s="8"/>
       <c r="U1578" s="8"/>
       <c r="V1578" s="48" t="s">
-        <v>1285</v>
+        <v>1284</v>
       </c>
     </row>
     <row r="1579" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -62007,7 +62007,7 @@
         <v>18</v>
       </c>
       <c r="V1588" s="36" t="s">
-        <v>1286</v>
+        <v>1285</v>
       </c>
     </row>
     <row r="1589" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -62417,7 +62417,7 @@
         <v>18</v>
       </c>
       <c r="V1599" s="5" t="s">
-        <v>1287</v>
+        <v>1286</v>
       </c>
     </row>
     <row r="1600" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -62708,7 +62708,7 @@
         <v>125</v>
       </c>
       <c r="N1607" s="16" t="s">
-        <v>1332</v>
+        <v>1330</v>
       </c>
       <c r="O1607" s="23" t="s">
         <v>0</v>
@@ -62717,7 +62717,7 @@
         <v>18</v>
       </c>
       <c r="V1607" s="36" t="s">
-        <v>1288</v>
+        <v>1287</v>
       </c>
     </row>
     <row r="1608" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -63039,7 +63039,7 @@
         <v>18</v>
       </c>
       <c r="V1616" s="36" t="s">
-        <v>1289</v>
+        <v>1288</v>
       </c>
     </row>
     <row r="1617" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -63369,7 +63369,7 @@
         <v>18</v>
       </c>
       <c r="V1625" s="5" t="s">
-        <v>1290</v>
+        <v>1289</v>
       </c>
     </row>
     <row r="1626" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -63783,8 +63783,8 @@
       <c r="P1637" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="V1637" s="63" t="s">
-        <v>1329</v>
+      <c r="V1637" s="62" t="s">
+        <v>1327</v>
       </c>
     </row>
     <row r="1638" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -63917,7 +63917,7 @@
       <c r="N1641" s="21" t="s">
         <v>901</v>
       </c>
-      <c r="O1641" s="62" t="s">
+      <c r="O1641" s="61" t="s">
         <v>1</v>
       </c>
       <c r="P1641" s="24"/>
@@ -64151,7 +64151,7 @@
         <v>1114</v>
       </c>
       <c r="V1647" s="5" t="s">
-        <v>1291</v>
+        <v>1290</v>
       </c>
     </row>
     <row r="1648" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -64475,7 +64475,7 @@
         <v>18</v>
       </c>
       <c r="V1656" s="5" t="s">
-        <v>1292</v>
+        <v>1291</v>
       </c>
     </row>
     <row r="1657" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -64795,7 +64795,7 @@
         <v>18</v>
       </c>
       <c r="V1665" s="36" t="s">
-        <v>1293</v>
+        <v>1292</v>
       </c>
     </row>
     <row r="1666" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -65144,7 +65144,7 @@
         <v>18</v>
       </c>
       <c r="V1675" s="36" t="s">
-        <v>1294</v>
+        <v>1293</v>
       </c>
     </row>
     <row r="1676" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -65410,7 +65410,7 @@
         <v>18</v>
       </c>
       <c r="V1683" s="36" t="s">
-        <v>1295</v>
+        <v>1294</v>
       </c>
     </row>
     <row r="1684" spans="3:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -65677,7 +65677,7 @@
         <v>898</v>
       </c>
       <c r="V1691" s="36" t="s">
-        <v>1296</v>
+        <v>1295</v>
       </c>
     </row>
     <row r="1692" spans="3:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -66042,7 +66042,7 @@
         <v>18</v>
       </c>
       <c r="V1702" s="36" t="s">
-        <v>1297</v>
+        <v>1296</v>
       </c>
     </row>
     <row r="1703" spans="3:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -66298,7 +66298,7 @@
         <v>898</v>
       </c>
       <c r="V1710" s="5" t="s">
-        <v>1296</v>
+        <v>1295</v>
       </c>
     </row>
     <row r="1711" spans="3:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -66901,7 +66901,7 @@
         <v>898</v>
       </c>
       <c r="V1729" s="5" t="s">
-        <v>1296</v>
+        <v>1295</v>
       </c>
     </row>
     <row r="1730" spans="3:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -67217,7 +67217,7 @@
         <v>18</v>
       </c>
       <c r="V1739" s="36" t="s">
-        <v>1298</v>
+        <v>1297</v>
       </c>
     </row>
     <row r="1740" spans="3:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -67470,7 +67470,7 @@
         <v>898</v>
       </c>
       <c r="V1747" s="5" t="s">
-        <v>1296</v>
+        <v>1295</v>
       </c>
     </row>
     <row r="1748" spans="3:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -67757,7 +67757,7 @@
         <v>18</v>
       </c>
       <c r="V1756" s="36" t="s">
-        <v>1299</v>
+        <v>1298</v>
       </c>
     </row>
     <row r="1757" spans="3:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -68040,7 +68040,7 @@
         <v>18</v>
       </c>
       <c r="V1765" s="36" t="s">
-        <v>1300</v>
+        <v>1299</v>
       </c>
     </row>
     <row r="1766" spans="3:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -68350,8 +68350,8 @@
       <c r="P1774" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="V1774" s="36" t="s">
-        <v>1301</v>
+      <c r="V1774" s="62" t="s">
+        <v>1339</v>
       </c>
     </row>
     <row r="1775" spans="3:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -68602,7 +68602,7 @@
         <v>18</v>
       </c>
       <c r="V1782" s="5" t="s">
-        <v>1300</v>
+        <v>1299</v>
       </c>
     </row>
     <row r="1783" spans="3:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -68922,7 +68922,7 @@
         <v>18</v>
       </c>
       <c r="V1792" s="5" t="s">
-        <v>1302</v>
+        <v>1300</v>
       </c>
     </row>
     <row r="1793" spans="3:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -69174,7 +69174,7 @@
         <v>18</v>
       </c>
       <c r="V1800" s="5" t="s">
-        <v>1300</v>
+        <v>1299</v>
       </c>
     </row>
     <row r="1801" spans="3:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -69398,7 +69398,7 @@
         <v>897</v>
       </c>
       <c r="V1807" s="5" t="s">
-        <v>1303</v>
+        <v>1301</v>
       </c>
     </row>
     <row r="1808" spans="3:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -69679,7 +69679,7 @@
         <v>18</v>
       </c>
       <c r="V1816" s="5" t="s">
-        <v>1300</v>
+        <v>1299</v>
       </c>
     </row>
     <row r="1817" spans="3:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -69936,7 +69936,7 @@
         <v>18</v>
       </c>
       <c r="V1824" s="5" t="s">
-        <v>1304</v>
+        <v>1302</v>
       </c>
     </row>
     <row r="1825" spans="3:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -70255,7 +70255,7 @@
         <v>18</v>
       </c>
       <c r="V1834" s="5" t="s">
-        <v>1300</v>
+        <v>1299</v>
       </c>
     </row>
     <row r="1835" spans="3:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -70478,7 +70478,7 @@
         <v>18</v>
       </c>
       <c r="V1841" s="5" t="s">
-        <v>1305</v>
+        <v>1303</v>
       </c>
     </row>
     <row r="1842" spans="3:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -70762,7 +70762,7 @@
         <v>18</v>
       </c>
       <c r="V1850" s="5" t="s">
-        <v>1300</v>
+        <v>1299</v>
       </c>
     </row>
     <row r="1851" spans="3:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -71120,7 +71120,7 @@
         <v>18</v>
       </c>
       <c r="V1861" s="36" t="s">
-        <v>1306</v>
+        <v>1304</v>
       </c>
     </row>
     <row r="1862" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -71372,7 +71372,7 @@
         <v>18</v>
       </c>
       <c r="V1869" s="5" t="s">
-        <v>1307</v>
+        <v>1305</v>
       </c>
     </row>
     <row r="1870" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -71621,7 +71621,7 @@
         <v>18</v>
       </c>
       <c r="V1877" s="5" t="s">
-        <v>1308</v>
+        <v>1306</v>
       </c>
     </row>
     <row r="1878" spans="3:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -71902,7 +71902,7 @@
         <v>18</v>
       </c>
       <c r="V1886" s="5" t="s">
-        <v>1307</v>
+        <v>1305</v>
       </c>
     </row>
     <row r="1887" spans="3:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -72248,7 +72248,7 @@
         <v>18</v>
       </c>
       <c r="V1897" s="5" t="s">
-        <v>1306</v>
+        <v>1304</v>
       </c>
     </row>
     <row r="1898" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -72503,7 +72503,7 @@
         <v>18</v>
       </c>
       <c r="V1905" s="36" t="s">
-        <v>1307</v>
+        <v>1305</v>
       </c>
     </row>
     <row r="1906" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -72708,7 +72708,7 @@
         <v>18</v>
       </c>
       <c r="V1911" s="36" t="s">
-        <v>1309</v>
+        <v>1307</v>
       </c>
     </row>
     <row r="1912" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -72992,7 +72992,7 @@
         <v>18</v>
       </c>
       <c r="V1920" s="5" t="s">
-        <v>1307</v>
+        <v>1305</v>
       </c>
     </row>
     <row r="1921" spans="3:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -73427,7 +73427,7 @@
         <v>18</v>
       </c>
       <c r="V1933" s="5" t="s">
-        <v>1310</v>
+        <v>1308</v>
       </c>
     </row>
     <row r="1934" spans="3:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -73460,7 +73460,7 @@
       </c>
       <c r="P1934" s="24"/>
       <c r="V1934" s="36" t="s">
-        <v>1311</v>
+        <v>1309</v>
       </c>
     </row>
     <row r="1935" spans="3:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -73691,7 +73691,7 @@
         <v>18</v>
       </c>
       <c r="V1941" s="36" t="s">
-        <v>1312</v>
+        <v>1310</v>
       </c>
     </row>
     <row r="1942" spans="3:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -73850,7 +73850,7 @@
       </c>
       <c r="P1946" s="24"/>
       <c r="V1946" s="36" t="s">
-        <v>1313</v>
+        <v>1311</v>
       </c>
     </row>
     <row r="1947" spans="3:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -73948,7 +73948,7 @@
         <v>898</v>
       </c>
       <c r="V1949" s="36" t="s">
-        <v>1296</v>
+        <v>1295</v>
       </c>
     </row>
     <row r="1950" spans="3:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -73981,7 +73981,7 @@
       </c>
       <c r="P1950" s="24"/>
       <c r="V1950" s="36" t="s">
-        <v>1314</v>
+        <v>1312</v>
       </c>
     </row>
     <row r="1951" spans="3:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -74014,7 +74014,7 @@
       </c>
       <c r="P1951" s="24"/>
       <c r="V1951" s="36" t="s">
-        <v>1315</v>
+        <v>1313</v>
       </c>
     </row>
     <row r="1952" spans="3:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -74140,7 +74140,7 @@
       </c>
       <c r="P1955" s="24"/>
       <c r="V1955" s="36" t="s">
-        <v>1316</v>
+        <v>1314</v>
       </c>
     </row>
     <row r="1956" spans="3:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -74236,7 +74236,7 @@
         <v>18</v>
       </c>
       <c r="V1958" s="5" t="s">
-        <v>1317</v>
+        <v>1315</v>
       </c>
     </row>
     <row r="1959" spans="3:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -74493,7 +74493,7 @@
         <v>898</v>
       </c>
       <c r="V1966" s="5" t="s">
-        <v>1296</v>
+        <v>1295</v>
       </c>
     </row>
     <row r="1967" spans="3:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -74830,7 +74830,7 @@
         <v>18</v>
       </c>
       <c r="V1976" s="5" t="s">
-        <v>1318</v>
+        <v>1316</v>
       </c>
     </row>
     <row r="1977" spans="3:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -74896,7 +74896,7 @@
         <v>303</v>
       </c>
       <c r="N1978" s="55" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="O1978" s="23" t="s">
         <v>1</v>
@@ -75502,7 +75502,7 @@
         <v>18</v>
       </c>
       <c r="V1996" s="5" t="s">
-        <v>1319</v>
+        <v>1317</v>
       </c>
     </row>
     <row r="1997" spans="3:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -75930,7 +75930,7 @@
         <v>18</v>
       </c>
       <c r="V2009" s="36" t="s">
-        <v>1320</v>
+        <v>1318</v>
       </c>
     </row>
     <row r="2010" spans="3:22" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
nmv 24 05 2024
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Padam Input Templates/TS 4.7 Padam Input Template.xlsx
+++ b/TS Jatai Working/Padam Input Templates/TS 4.7 Padam Input Template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ALL IMP DATA\GitHub\texts\TS Jatai Working\Padam Input Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8273619-2DA4-451D-A329-CF3B1542D161}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6042C03-4221-47EE-B74B-40B2830E6977}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3810,9 +3810,6 @@
     <t xml:space="preserve">puqrAqNA iti# purAqNAH </t>
   </si>
   <si>
-    <t xml:space="preserve">RuqtAvetyRuqtA - vAq </t>
-  </si>
-  <si>
     <t xml:space="preserve">niSha#ttaq itiq ni - saqttaqH </t>
   </si>
   <si>
@@ -4048,6 +4045,9 @@
   </si>
   <si>
     <t xml:space="preserve">dUqShayaqnniti# dUqShayann# </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RuqtAvetyRuqta - vAq </t>
   </si>
 </sst>
 </file>
@@ -4431,7 +4431,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4715,9 +4715,9 @@
   <dimension ref="A1:W2010"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="I1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1762" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A1288" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="H1" sqref="H1"/>
-      <selection pane="bottomLeft" activeCell="N1774" sqref="N1774"/>
+      <selection pane="bottomLeft" activeCell="T1302" sqref="T1302"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -5276,7 +5276,7 @@
         <v>1</v>
       </c>
       <c r="N2" s="21" t="s">
-        <v>1319</v>
+        <v>1318</v>
       </c>
       <c r="O2" s="23" t="s">
         <v>16</v>
@@ -5526,7 +5526,7 @@
         <v>7</v>
       </c>
       <c r="N8" s="55" t="s">
-        <v>1321</v>
+        <v>1320</v>
       </c>
       <c r="O8" s="23"/>
       <c r="P8" s="23"/>
@@ -13811,7 +13811,7 @@
       <c r="T243" s="8"/>
       <c r="U243" s="8"/>
       <c r="V243" s="63" t="s">
-        <v>1326</v>
+        <v>1325</v>
       </c>
     </row>
     <row r="244" spans="9:22" s="6" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -15687,7 +15687,7 @@
         <v>67</v>
       </c>
       <c r="N300" s="55" t="s">
-        <v>1322</v>
+        <v>1321</v>
       </c>
       <c r="O300" s="23"/>
       <c r="P300" s="23"/>
@@ -29821,7 +29821,7 @@
       <c r="T726" s="8"/>
       <c r="U726" s="8"/>
       <c r="V726" s="57" t="s">
-        <v>1323</v>
+        <v>1322</v>
       </c>
     </row>
     <row r="727" spans="9:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -29922,7 +29922,7 @@
       <c r="T729" s="8"/>
       <c r="U729" s="8"/>
       <c r="V729" s="62" t="s">
-        <v>1332</v>
+        <v>1331</v>
       </c>
     </row>
     <row r="730" spans="9:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -32219,7 +32219,7 @@
       <c r="T798" s="8"/>
       <c r="U798" s="8"/>
       <c r="V798" s="62" t="s">
-        <v>1333</v>
+        <v>1332</v>
       </c>
     </row>
     <row r="799" spans="9:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -36234,7 +36234,7 @@
       <c r="T917" s="8"/>
       <c r="U917" s="8"/>
       <c r="V917" s="62" t="s">
-        <v>1331</v>
+        <v>1330</v>
       </c>
     </row>
     <row r="918" spans="9:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -39545,7 +39545,7 @@
       <c r="T1016" s="8"/>
       <c r="U1016" s="8"/>
       <c r="V1016" s="54" t="s">
-        <v>1320</v>
+        <v>1319</v>
       </c>
     </row>
     <row r="1017" spans="9:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -41502,7 +41502,7 @@
         <v>898</v>
       </c>
       <c r="V1074" s="62" t="s">
-        <v>1334</v>
+        <v>1333</v>
       </c>
     </row>
     <row r="1075" spans="5:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -48782,7 +48782,7 @@
         <v>909</v>
       </c>
       <c r="T1259" s="56" t="s">
-        <v>1324</v>
+        <v>1323</v>
       </c>
       <c r="U1259" s="8"/>
       <c r="V1259" s="5" t="s">
@@ -49997,8 +49997,8 @@
       <c r="S1289" s="8"/>
       <c r="T1289" s="8"/>
       <c r="U1289" s="8"/>
-      <c r="V1289" s="36" t="s">
-        <v>1260</v>
+      <c r="V1289" s="62" t="s">
+        <v>1339</v>
       </c>
     </row>
     <row r="1290" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -50317,7 +50317,7 @@
       <c r="T1297" s="8"/>
       <c r="U1297" s="8"/>
       <c r="V1297" s="36" t="s">
-        <v>1261</v>
+        <v>1260</v>
       </c>
     </row>
     <row r="1298" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -50423,7 +50423,7 @@
         <f t="shared" si="82"/>
         <v>55</v>
       </c>
-      <c r="N1300" s="21" t="s">
+      <c r="N1300" s="16" t="s">
         <v>321</v>
       </c>
       <c r="O1300" s="23"/>
@@ -50750,7 +50750,7 @@
       <c r="T1308" s="8"/>
       <c r="U1308" s="8"/>
       <c r="V1308" s="36" t="s">
-        <v>1262</v>
+        <v>1261</v>
       </c>
     </row>
     <row r="1309" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -51074,7 +51074,7 @@
         <v>898</v>
       </c>
       <c r="V1316" s="5" t="s">
-        <v>1263</v>
+        <v>1262</v>
       </c>
     </row>
     <row r="1317" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -51546,7 +51546,7 @@
       <c r="T1328" s="8"/>
       <c r="U1328" s="8"/>
       <c r="V1328" s="36" t="s">
-        <v>1264</v>
+        <v>1263</v>
       </c>
     </row>
     <row r="1329" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -51860,7 +51860,7 @@
       <c r="T1336" s="8"/>
       <c r="U1336" s="8"/>
       <c r="V1336" s="5" t="s">
-        <v>1265</v>
+        <v>1264</v>
       </c>
     </row>
     <row r="1337" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -52065,7 +52065,7 @@
       <c r="T1341" s="8"/>
       <c r="U1341" s="8"/>
       <c r="V1341" s="62" t="s">
-        <v>1338</v>
+        <v>1337</v>
       </c>
     </row>
     <row r="1342" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -52423,7 +52423,7 @@
       <c r="T1350" s="8"/>
       <c r="U1350" s="8"/>
       <c r="V1350" s="62" t="s">
-        <v>1336</v>
+        <v>1335</v>
       </c>
     </row>
     <row r="1351" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -52876,7 +52876,7 @@
       <c r="T1361" s="8"/>
       <c r="U1361" s="8"/>
       <c r="V1361" s="37" t="s">
-        <v>1266</v>
+        <v>1265</v>
       </c>
     </row>
     <row r="1362" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -53270,7 +53270,7 @@
       <c r="T1371" s="8"/>
       <c r="U1371" s="8"/>
       <c r="V1371" s="62" t="s">
-        <v>1328</v>
+        <v>1327</v>
       </c>
     </row>
     <row r="1372" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -53649,7 +53649,7 @@
       <c r="T1380" s="8"/>
       <c r="U1380" s="8"/>
       <c r="V1380" s="5" t="s">
-        <v>1267</v>
+        <v>1266</v>
       </c>
     </row>
     <row r="1381" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -54004,7 +54004,7 @@
       <c r="T1389" s="8"/>
       <c r="U1389" s="8"/>
       <c r="V1389" s="5" t="s">
-        <v>1268</v>
+        <v>1267</v>
       </c>
     </row>
     <row r="1390" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -54123,7 +54123,7 @@
       <c r="T1392" s="8"/>
       <c r="U1392" s="8"/>
       <c r="V1392" s="62" t="s">
-        <v>1337</v>
+        <v>1336</v>
       </c>
     </row>
     <row r="1393" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -54323,7 +54323,7 @@
       <c r="T1397" s="8"/>
       <c r="U1397" s="8"/>
       <c r="V1397" s="5" t="s">
-        <v>1269</v>
+        <v>1268</v>
       </c>
     </row>
     <row r="1398" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -54616,7 +54616,7 @@
       <c r="T1404" s="8"/>
       <c r="U1404" s="8"/>
       <c r="V1404" s="36" t="s">
-        <v>1270</v>
+        <v>1269</v>
       </c>
     </row>
     <row r="1405" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -54933,7 +54933,7 @@
       <c r="T1412" s="8"/>
       <c r="U1412" s="8"/>
       <c r="V1412" s="5" t="s">
-        <v>1271</v>
+        <v>1270</v>
       </c>
     </row>
     <row r="1413" spans="1:23" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -55383,7 +55383,7 @@
       <c r="T1423" s="8"/>
       <c r="U1423" s="8"/>
       <c r="V1423" s="5" t="s">
-        <v>1272</v>
+        <v>1271</v>
       </c>
     </row>
     <row r="1424" spans="1:23" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -55753,7 +55753,7 @@
       <c r="T1432" s="8"/>
       <c r="U1432" s="8"/>
       <c r="V1432" s="5" t="s">
-        <v>1273</v>
+        <v>1272</v>
       </c>
     </row>
     <row r="1433" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -56329,7 +56329,7 @@
       <c r="T1446" s="8"/>
       <c r="U1446" s="8"/>
       <c r="V1446" s="62" t="s">
-        <v>1329</v>
+        <v>1328</v>
       </c>
     </row>
     <row r="1447" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -57122,7 +57122,7 @@
       <c r="T1466" s="8"/>
       <c r="U1466" s="8"/>
       <c r="V1466" s="5" t="s">
-        <v>1274</v>
+        <v>1273</v>
       </c>
     </row>
     <row r="1467" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -57411,7 +57411,7 @@
         <v>897</v>
       </c>
       <c r="V1473" s="5" t="s">
-        <v>1275</v>
+        <v>1274</v>
       </c>
     </row>
     <row r="1474" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -57770,7 +57770,7 @@
       <c r="T1482" s="8"/>
       <c r="U1482" s="8"/>
       <c r="V1482" s="5" t="s">
-        <v>1276</v>
+        <v>1275</v>
       </c>
     </row>
     <row r="1483" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -58179,7 +58179,7 @@
       <c r="T1492" s="8"/>
       <c r="U1492" s="8"/>
       <c r="V1492" s="5" t="s">
-        <v>1277</v>
+        <v>1276</v>
       </c>
     </row>
     <row r="1493" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -58497,7 +58497,7 @@
       <c r="T1500" s="8"/>
       <c r="U1500" s="8"/>
       <c r="V1500" s="5" t="s">
-        <v>1278</v>
+        <v>1277</v>
       </c>
     </row>
     <row r="1501" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -58735,7 +58735,7 @@
       <c r="T1506" s="8"/>
       <c r="U1506" s="8"/>
       <c r="V1506" s="62" t="s">
-        <v>1335</v>
+        <v>1334</v>
       </c>
     </row>
     <row r="1507" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -58854,7 +58854,7 @@
       <c r="T1509" s="8"/>
       <c r="U1509" s="8"/>
       <c r="V1509" s="5" t="s">
-        <v>1279</v>
+        <v>1278</v>
       </c>
     </row>
     <row r="1510" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -59270,7 +59270,7 @@
         <v>897</v>
       </c>
       <c r="V1519" s="5" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
     </row>
     <row r="1520" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -59981,7 +59981,7 @@
       <c r="T1537" s="8"/>
       <c r="U1537" s="8"/>
       <c r="V1537" s="36" t="s">
-        <v>1281</v>
+        <v>1280</v>
       </c>
     </row>
     <row r="1538" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -60377,7 +60377,7 @@
         <v>897</v>
       </c>
       <c r="V1547" s="36" t="s">
-        <v>1282</v>
+        <v>1281</v>
       </c>
     </row>
     <row r="1548" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -61255,7 +61255,7 @@
       <c r="T1568" s="8"/>
       <c r="U1568" s="8"/>
       <c r="V1568" s="36" t="s">
-        <v>1283</v>
+        <v>1282</v>
       </c>
     </row>
     <row r="1569" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -61649,7 +61649,7 @@
       <c r="T1578" s="8"/>
       <c r="U1578" s="8"/>
       <c r="V1578" s="48" t="s">
-        <v>1284</v>
+        <v>1283</v>
       </c>
     </row>
     <row r="1579" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -62007,7 +62007,7 @@
         <v>18</v>
       </c>
       <c r="V1588" s="36" t="s">
-        <v>1285</v>
+        <v>1284</v>
       </c>
     </row>
     <row r="1589" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -62417,7 +62417,7 @@
         <v>18</v>
       </c>
       <c r="V1599" s="5" t="s">
-        <v>1286</v>
+        <v>1285</v>
       </c>
     </row>
     <row r="1600" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -62708,7 +62708,7 @@
         <v>125</v>
       </c>
       <c r="N1607" s="16" t="s">
-        <v>1330</v>
+        <v>1329</v>
       </c>
       <c r="O1607" s="23" t="s">
         <v>0</v>
@@ -62717,7 +62717,7 @@
         <v>18</v>
       </c>
       <c r="V1607" s="36" t="s">
-        <v>1287</v>
+        <v>1286</v>
       </c>
     </row>
     <row r="1608" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -63039,7 +63039,7 @@
         <v>18</v>
       </c>
       <c r="V1616" s="36" t="s">
-        <v>1288</v>
+        <v>1287</v>
       </c>
     </row>
     <row r="1617" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -63369,7 +63369,7 @@
         <v>18</v>
       </c>
       <c r="V1625" s="5" t="s">
-        <v>1289</v>
+        <v>1288</v>
       </c>
     </row>
     <row r="1626" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -63784,7 +63784,7 @@
         <v>18</v>
       </c>
       <c r="V1637" s="62" t="s">
-        <v>1327</v>
+        <v>1326</v>
       </c>
     </row>
     <row r="1638" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -64151,7 +64151,7 @@
         <v>1114</v>
       </c>
       <c r="V1647" s="5" t="s">
-        <v>1290</v>
+        <v>1289</v>
       </c>
     </row>
     <row r="1648" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -64475,7 +64475,7 @@
         <v>18</v>
       </c>
       <c r="V1656" s="5" t="s">
-        <v>1291</v>
+        <v>1290</v>
       </c>
     </row>
     <row r="1657" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -64795,7 +64795,7 @@
         <v>18</v>
       </c>
       <c r="V1665" s="36" t="s">
-        <v>1292</v>
+        <v>1291</v>
       </c>
     </row>
     <row r="1666" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -65144,7 +65144,7 @@
         <v>18</v>
       </c>
       <c r="V1675" s="36" t="s">
-        <v>1293</v>
+        <v>1292</v>
       </c>
     </row>
     <row r="1676" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -65410,7 +65410,7 @@
         <v>18</v>
       </c>
       <c r="V1683" s="36" t="s">
-        <v>1294</v>
+        <v>1293</v>
       </c>
     </row>
     <row r="1684" spans="3:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -65677,7 +65677,7 @@
         <v>898</v>
       </c>
       <c r="V1691" s="36" t="s">
-        <v>1295</v>
+        <v>1294</v>
       </c>
     </row>
     <row r="1692" spans="3:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -66042,7 +66042,7 @@
         <v>18</v>
       </c>
       <c r="V1702" s="36" t="s">
-        <v>1296</v>
+        <v>1295</v>
       </c>
     </row>
     <row r="1703" spans="3:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -66298,7 +66298,7 @@
         <v>898</v>
       </c>
       <c r="V1710" s="5" t="s">
-        <v>1295</v>
+        <v>1294</v>
       </c>
     </row>
     <row r="1711" spans="3:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -66901,7 +66901,7 @@
         <v>898</v>
       </c>
       <c r="V1729" s="5" t="s">
-        <v>1295</v>
+        <v>1294</v>
       </c>
     </row>
     <row r="1730" spans="3:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -67217,7 +67217,7 @@
         <v>18</v>
       </c>
       <c r="V1739" s="36" t="s">
-        <v>1297</v>
+        <v>1296</v>
       </c>
     </row>
     <row r="1740" spans="3:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -67470,7 +67470,7 @@
         <v>898</v>
       </c>
       <c r="V1747" s="5" t="s">
-        <v>1295</v>
+        <v>1294</v>
       </c>
     </row>
     <row r="1748" spans="3:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -67757,7 +67757,7 @@
         <v>18</v>
       </c>
       <c r="V1756" s="36" t="s">
-        <v>1298</v>
+        <v>1297</v>
       </c>
     </row>
     <row r="1757" spans="3:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -68040,7 +68040,7 @@
         <v>18</v>
       </c>
       <c r="V1765" s="36" t="s">
-        <v>1299</v>
+        <v>1298</v>
       </c>
     </row>
     <row r="1766" spans="3:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -68351,7 +68351,7 @@
         <v>18</v>
       </c>
       <c r="V1774" s="62" t="s">
-        <v>1339</v>
+        <v>1338</v>
       </c>
     </row>
     <row r="1775" spans="3:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -68602,7 +68602,7 @@
         <v>18</v>
       </c>
       <c r="V1782" s="5" t="s">
-        <v>1299</v>
+        <v>1298</v>
       </c>
     </row>
     <row r="1783" spans="3:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -68922,7 +68922,7 @@
         <v>18</v>
       </c>
       <c r="V1792" s="5" t="s">
-        <v>1300</v>
+        <v>1299</v>
       </c>
     </row>
     <row r="1793" spans="3:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -69174,7 +69174,7 @@
         <v>18</v>
       </c>
       <c r="V1800" s="5" t="s">
-        <v>1299</v>
+        <v>1298</v>
       </c>
     </row>
     <row r="1801" spans="3:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -69398,7 +69398,7 @@
         <v>897</v>
       </c>
       <c r="V1807" s="5" t="s">
-        <v>1301</v>
+        <v>1300</v>
       </c>
     </row>
     <row r="1808" spans="3:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -69679,7 +69679,7 @@
         <v>18</v>
       </c>
       <c r="V1816" s="5" t="s">
-        <v>1299</v>
+        <v>1298</v>
       </c>
     </row>
     <row r="1817" spans="3:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -69936,7 +69936,7 @@
         <v>18</v>
       </c>
       <c r="V1824" s="5" t="s">
-        <v>1302</v>
+        <v>1301</v>
       </c>
     </row>
     <row r="1825" spans="3:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -70255,7 +70255,7 @@
         <v>18</v>
       </c>
       <c r="V1834" s="5" t="s">
-        <v>1299</v>
+        <v>1298</v>
       </c>
     </row>
     <row r="1835" spans="3:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -70478,7 +70478,7 @@
         <v>18</v>
       </c>
       <c r="V1841" s="5" t="s">
-        <v>1303</v>
+        <v>1302</v>
       </c>
     </row>
     <row r="1842" spans="3:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -70762,7 +70762,7 @@
         <v>18</v>
       </c>
       <c r="V1850" s="5" t="s">
-        <v>1299</v>
+        <v>1298</v>
       </c>
     </row>
     <row r="1851" spans="3:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -71120,7 +71120,7 @@
         <v>18</v>
       </c>
       <c r="V1861" s="36" t="s">
-        <v>1304</v>
+        <v>1303</v>
       </c>
     </row>
     <row r="1862" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -71372,7 +71372,7 @@
         <v>18</v>
       </c>
       <c r="V1869" s="5" t="s">
-        <v>1305</v>
+        <v>1304</v>
       </c>
     </row>
     <row r="1870" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -71621,7 +71621,7 @@
         <v>18</v>
       </c>
       <c r="V1877" s="5" t="s">
-        <v>1306</v>
+        <v>1305</v>
       </c>
     </row>
     <row r="1878" spans="3:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -71902,7 +71902,7 @@
         <v>18</v>
       </c>
       <c r="V1886" s="5" t="s">
-        <v>1305</v>
+        <v>1304</v>
       </c>
     </row>
     <row r="1887" spans="3:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -72248,7 +72248,7 @@
         <v>18</v>
       </c>
       <c r="V1897" s="5" t="s">
-        <v>1304</v>
+        <v>1303</v>
       </c>
     </row>
     <row r="1898" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -72503,7 +72503,7 @@
         <v>18</v>
       </c>
       <c r="V1905" s="36" t="s">
-        <v>1305</v>
+        <v>1304</v>
       </c>
     </row>
     <row r="1906" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -72708,7 +72708,7 @@
         <v>18</v>
       </c>
       <c r="V1911" s="36" t="s">
-        <v>1307</v>
+        <v>1306</v>
       </c>
     </row>
     <row r="1912" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -72992,7 +72992,7 @@
         <v>18</v>
       </c>
       <c r="V1920" s="5" t="s">
-        <v>1305</v>
+        <v>1304</v>
       </c>
     </row>
     <row r="1921" spans="3:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -73427,7 +73427,7 @@
         <v>18</v>
       </c>
       <c r="V1933" s="5" t="s">
-        <v>1308</v>
+        <v>1307</v>
       </c>
     </row>
     <row r="1934" spans="3:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -73460,7 +73460,7 @@
       </c>
       <c r="P1934" s="24"/>
       <c r="V1934" s="36" t="s">
-        <v>1309</v>
+        <v>1308</v>
       </c>
     </row>
     <row r="1935" spans="3:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -73691,7 +73691,7 @@
         <v>18</v>
       </c>
       <c r="V1941" s="36" t="s">
-        <v>1310</v>
+        <v>1309</v>
       </c>
     </row>
     <row r="1942" spans="3:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -73850,7 +73850,7 @@
       </c>
       <c r="P1946" s="24"/>
       <c r="V1946" s="36" t="s">
-        <v>1311</v>
+        <v>1310</v>
       </c>
     </row>
     <row r="1947" spans="3:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -73948,7 +73948,7 @@
         <v>898</v>
       </c>
       <c r="V1949" s="36" t="s">
-        <v>1295</v>
+        <v>1294</v>
       </c>
     </row>
     <row r="1950" spans="3:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -73981,7 +73981,7 @@
       </c>
       <c r="P1950" s="24"/>
       <c r="V1950" s="36" t="s">
-        <v>1312</v>
+        <v>1311</v>
       </c>
     </row>
     <row r="1951" spans="3:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -74014,7 +74014,7 @@
       </c>
       <c r="P1951" s="24"/>
       <c r="V1951" s="36" t="s">
-        <v>1313</v>
+        <v>1312</v>
       </c>
     </row>
     <row r="1952" spans="3:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -74140,7 +74140,7 @@
       </c>
       <c r="P1955" s="24"/>
       <c r="V1955" s="36" t="s">
-        <v>1314</v>
+        <v>1313</v>
       </c>
     </row>
     <row r="1956" spans="3:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -74236,7 +74236,7 @@
         <v>18</v>
       </c>
       <c r="V1958" s="5" t="s">
-        <v>1315</v>
+        <v>1314</v>
       </c>
     </row>
     <row r="1959" spans="3:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -74493,7 +74493,7 @@
         <v>898</v>
       </c>
       <c r="V1966" s="5" t="s">
-        <v>1295</v>
+        <v>1294</v>
       </c>
     </row>
     <row r="1967" spans="3:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -74830,7 +74830,7 @@
         <v>18</v>
       </c>
       <c r="V1976" s="5" t="s">
-        <v>1316</v>
+        <v>1315</v>
       </c>
     </row>
     <row r="1977" spans="3:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -74896,7 +74896,7 @@
         <v>303</v>
       </c>
       <c r="N1978" s="55" t="s">
-        <v>1325</v>
+        <v>1324</v>
       </c>
       <c r="O1978" s="23" t="s">
         <v>1</v>
@@ -75502,7 +75502,7 @@
         <v>18</v>
       </c>
       <c r="V1996" s="5" t="s">
-        <v>1317</v>
+        <v>1316</v>
       </c>
     </row>
     <row r="1997" spans="3:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -75930,7 +75930,7 @@
         <v>18</v>
       </c>
       <c r="V2009" s="36" t="s">
-        <v>1318</v>
+        <v>1317</v>
       </c>
     </row>
     <row r="2010" spans="3:22" x14ac:dyDescent="0.25">

</xml_diff>